<commit_message>
Graph polish and grand summarise  / if else fix
</commit_message>
<xml_diff>
--- a/Output/AcqTrends/CSIS_DoD_DIB_Trends.xlsx
+++ b/Output/AcqTrends/CSIS_DoD_DIB_Trends.xlsx
@@ -215,19 +215,19 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="14">
     <numFmt numFmtId="169" formatCode="0.00,&quot;K&quot;"/>
-    <numFmt numFmtId="235" formatCode="0.00,&quot;K&quot;"/>
+    <numFmt numFmtId="253" formatCode="0.00,&quot;K&quot;"/>
     <numFmt numFmtId="201" formatCode="0.00,&quot;K&quot;"/>
     <numFmt numFmtId="237" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="175" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="202" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="206" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="249" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="252" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="244" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="247" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="213" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="242" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="250" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="251" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="254" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -266,20 +266,20 @@
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="235" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="253" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="201" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="237" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="175" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="202" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="206" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="249" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="252" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="244" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="247" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="213" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="242" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="250" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="251" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="254" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1880,58 +1880,58 @@
       <c r="N2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="5" t="n">
+      <c r="O2" s="15" t="n">
         <v>1607832650.0848</v>
       </c>
-      <c r="P2" s="5" t="n">
+      <c r="P2" s="15" t="n">
         <v>1751871558.4642</v>
       </c>
-      <c r="Q2" s="5" t="n">
+      <c r="Q2" s="15" t="n">
         <v>1506361369.1731</v>
       </c>
-      <c r="R2" s="5" t="n">
+      <c r="R2" s="15" t="n">
         <v>1396531382.5087</v>
       </c>
-      <c r="S2" s="5" t="n">
+      <c r="S2" s="15" t="n">
         <v>1397976506.2712</v>
       </c>
-      <c r="T2" s="5" t="n">
+      <c r="T2" s="15" t="n">
         <v>1279752259.8247</v>
       </c>
-      <c r="U2" s="5" t="n">
+      <c r="U2" s="15" t="n">
         <v>1049133781.4795</v>
       </c>
-      <c r="V2" s="5" t="n">
+      <c r="V2" s="15" t="n">
         <v>1073603566.7955</v>
       </c>
-      <c r="W2" s="5" t="n">
+      <c r="W2" s="15" t="n">
         <v>1048450862.5594</v>
       </c>
-      <c r="X2" s="5" t="n">
+      <c r="X2" s="15" t="n">
         <v>1088102147.7351</v>
       </c>
-      <c r="Y2" s="5" t="n">
+      <c r="Y2" s="15" t="n">
         <v>1072746922.942</v>
       </c>
-      <c r="Z2" s="5" t="n">
+      <c r="Z2" s="15" t="n">
         <v>1096865763.5188</v>
       </c>
-      <c r="AA2" s="5" t="n">
+      <c r="AA2" s="15" t="n">
         <v>1188706092.6348</v>
       </c>
-      <c r="AB2" s="5" t="n">
+      <c r="AB2" s="15" t="n">
         <v>926769387.3954</v>
       </c>
-      <c r="AC2" s="5" t="n">
+      <c r="AC2" s="15" t="n">
         <v>976003450.1165</v>
       </c>
-      <c r="AD2" s="5" t="n">
+      <c r="AD2" s="15" t="n">
         <v>983305068.5037</v>
       </c>
-      <c r="AE2" s="5" t="n">
+      <c r="AE2" s="15" t="n">
         <v>926451906.4684</v>
       </c>
-      <c r="AF2" s="5" t="n">
+      <c r="AF2" s="15" t="n">
         <v>1096865763.5188</v>
       </c>
       <c r="AG2" s="7" t="n">
@@ -1994,58 +1994,58 @@
       <c r="N3" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="O3" s="5" t="n">
+      <c r="O3" s="15" t="n">
         <v>1184454239.6496</v>
       </c>
-      <c r="P3" s="5" t="n">
+      <c r="P3" s="15" t="n">
         <v>1228271132.5837</v>
       </c>
-      <c r="Q3" s="5" t="n">
+      <c r="Q3" s="15" t="n">
         <v>1140495002.7928</v>
       </c>
-      <c r="R3" s="5" t="n">
+      <c r="R3" s="15" t="n">
         <v>1024201877.6785</v>
       </c>
-      <c r="S3" s="5" t="n">
+      <c r="S3" s="15" t="n">
         <v>896870805.4232</v>
       </c>
-      <c r="T3" s="5" t="n">
+      <c r="T3" s="15" t="n">
         <v>960414796.0546</v>
       </c>
-      <c r="U3" s="5" t="n">
+      <c r="U3" s="15" t="n">
         <v>878985475.2202</v>
       </c>
-      <c r="V3" s="5" t="n">
+      <c r="V3" s="15" t="n">
         <v>751928698.974</v>
       </c>
-      <c r="W3" s="5" t="n">
+      <c r="W3" s="15" t="n">
         <v>815327907.857</v>
       </c>
-      <c r="X3" s="5" t="n">
+      <c r="X3" s="15" t="n">
         <v>844568319.4829</v>
       </c>
-      <c r="Y3" s="5" t="n">
+      <c r="Y3" s="15" t="n">
         <v>787108243.3135</v>
       </c>
-      <c r="Z3" s="5" t="n">
+      <c r="Z3" s="15" t="n">
         <v>820630788.2635</v>
       </c>
-      <c r="AA3" s="5" t="n">
+      <c r="AA3" s="15" t="n">
         <v>686536567.6669</v>
       </c>
-      <c r="AB3" s="5" t="n">
+      <c r="AB3" s="15" t="n">
         <v>545764074.6504</v>
       </c>
-      <c r="AC3" s="5" t="n">
+      <c r="AC3" s="15" t="n">
         <v>564021752.7514</v>
       </c>
-      <c r="AD3" s="5" t="n">
+      <c r="AD3" s="15" t="n">
         <v>783509578.311</v>
       </c>
-      <c r="AE3" s="5" t="n">
+      <c r="AE3" s="15" t="n">
         <v>704578096.1892</v>
       </c>
-      <c r="AF3" s="5" t="n">
+      <c r="AF3" s="15" t="n">
         <v>820630788.2635</v>
       </c>
       <c r="AG3" s="7" t="n">
@@ -2108,58 +2108,58 @@
       <c r="N4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="5" t="n">
+      <c r="O4" s="15" t="n">
         <v>6058548489.082</v>
       </c>
-      <c r="P4" s="5" t="n">
+      <c r="P4" s="15" t="n">
         <v>6080450819.0119</v>
       </c>
-      <c r="Q4" s="5" t="n">
+      <c r="Q4" s="15" t="n">
         <v>6779332127.7524</v>
       </c>
-      <c r="R4" s="5" t="n">
+      <c r="R4" s="15" t="n">
         <v>6093289597.1129</v>
       </c>
-      <c r="S4" s="5" t="n">
+      <c r="S4" s="15" t="n">
         <v>5262222494.4274</v>
       </c>
-      <c r="T4" s="5" t="n">
+      <c r="T4" s="15" t="n">
         <v>5079840604.2751</v>
       </c>
-      <c r="U4" s="5" t="n">
+      <c r="U4" s="15" t="n">
         <v>3567145813.244</v>
       </c>
-      <c r="V4" s="5" t="n">
+      <c r="V4" s="15" t="n">
         <v>4141995592.0904</v>
       </c>
-      <c r="W4" s="5" t="n">
+      <c r="W4" s="15" t="n">
         <v>3565259691.7783</v>
       </c>
-      <c r="X4" s="5" t="n">
+      <c r="X4" s="15" t="n">
         <v>3492208221.3053</v>
       </c>
-      <c r="Y4" s="5" t="n">
+      <c r="Y4" s="15" t="n">
         <v>3649991757.8593</v>
       </c>
-      <c r="Z4" s="5" t="n">
+      <c r="Z4" s="15" t="n">
         <v>3901328619.9928</v>
       </c>
-      <c r="AA4" s="5" t="n">
+      <c r="AA4" s="15" t="n">
         <v>3830751102.3953</v>
       </c>
-      <c r="AB4" s="5" t="n">
+      <c r="AB4" s="15" t="n">
         <v>4021172451.8518</v>
       </c>
-      <c r="AC4" s="5" t="n">
+      <c r="AC4" s="15" t="n">
         <v>3517341896.4453</v>
       </c>
-      <c r="AD4" s="5" t="n">
+      <c r="AD4" s="15" t="n">
         <v>3678372019.6405</v>
       </c>
-      <c r="AE4" s="5" t="n">
+      <c r="AE4" s="15" t="n">
         <v>3920322861.3483</v>
       </c>
-      <c r="AF4" s="5" t="n">
+      <c r="AF4" s="15" t="n">
         <v>3901328619.9928</v>
       </c>
       <c r="AG4" s="7" t="n">
@@ -2222,58 +2222,58 @@
       <c r="N5" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="O5" s="5" t="n">
+      <c r="O5" s="15" t="n">
         <v>5679433896.1785</v>
       </c>
-      <c r="P5" s="5" t="n">
+      <c r="P5" s="15" t="n">
         <v>5624659404.6315</v>
       </c>
-      <c r="Q5" s="5" t="n">
+      <c r="Q5" s="15" t="n">
         <v>5212638422.3091</v>
       </c>
-      <c r="R5" s="5" t="n">
+      <c r="R5" s="15" t="n">
         <v>6288316411.3781</v>
       </c>
-      <c r="S5" s="5" t="n">
+      <c r="S5" s="15" t="n">
         <v>5657555259.5043</v>
       </c>
-      <c r="T5" s="5" t="n">
+      <c r="T5" s="15" t="n">
         <v>3904127512.8452</v>
       </c>
-      <c r="U5" s="5" t="n">
+      <c r="U5" s="15" t="n">
         <v>3157315866.5217</v>
       </c>
-      <c r="V5" s="5" t="n">
+      <c r="V5" s="15" t="n">
         <v>2692614083.0845</v>
       </c>
-      <c r="W5" s="5" t="n">
+      <c r="W5" s="15" t="n">
         <v>3128570143.1366</v>
       </c>
-      <c r="X5" s="5" t="n">
+      <c r="X5" s="15" t="n">
         <v>3199159154.8128</v>
       </c>
-      <c r="Y5" s="5" t="n">
+      <c r="Y5" s="15" t="n">
         <v>3037857677.0835</v>
       </c>
-      <c r="Z5" s="5" t="n">
+      <c r="Z5" s="15" t="n">
         <v>3446915761.444</v>
       </c>
-      <c r="AA5" s="5" t="n">
+      <c r="AA5" s="15" t="n">
         <v>3536696065.3334</v>
       </c>
-      <c r="AB5" s="5" t="n">
+      <c r="AB5" s="15" t="n">
         <v>3005062231.913</v>
       </c>
-      <c r="AC5" s="5" t="n">
+      <c r="AC5" s="15" t="n">
         <v>3052114457.93</v>
       </c>
-      <c r="AD5" s="5" t="n">
+      <c r="AD5" s="15" t="n">
         <v>3359581254.4839</v>
       </c>
-      <c r="AE5" s="5" t="n">
+      <c r="AE5" s="15" t="n">
         <v>3618751504.3042</v>
       </c>
-      <c r="AF5" s="5" t="n">
+      <c r="AF5" s="15" t="n">
         <v>3446915761.444</v>
       </c>
       <c r="AG5" s="7" t="n">
@@ -2336,58 +2336,58 @@
       <c r="N6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O6" s="5" t="n">
+      <c r="O6" s="15" t="n">
         <v>3741321610.9336</v>
       </c>
-      <c r="P6" s="5" t="n">
+      <c r="P6" s="15" t="n">
         <v>3625952821.6054</v>
       </c>
-      <c r="Q6" s="5" t="n">
+      <c r="Q6" s="15" t="n">
         <v>3149991887.2102</v>
       </c>
-      <c r="R6" s="5" t="n">
+      <c r="R6" s="15" t="n">
         <v>2991291521.2622</v>
       </c>
-      <c r="S6" s="5" t="n">
+      <c r="S6" s="15" t="n">
         <v>3048040619.9372</v>
       </c>
-      <c r="T6" s="5" t="n">
+      <c r="T6" s="15" t="n">
         <v>2474472259.8299</v>
       </c>
-      <c r="U6" s="5" t="n">
+      <c r="U6" s="15" t="n">
         <v>1960743379.2061</v>
       </c>
-      <c r="V6" s="5" t="n">
+      <c r="V6" s="15" t="n">
         <v>2086527003.9821</v>
       </c>
-      <c r="W6" s="5" t="n">
+      <c r="W6" s="15" t="n">
         <v>1929095879.8002</v>
       </c>
-      <c r="X6" s="5" t="n">
+      <c r="X6" s="15" t="n">
         <v>1907797922.1413</v>
       </c>
-      <c r="Y6" s="5" t="n">
+      <c r="Y6" s="15" t="n">
         <v>1867693420.1991</v>
       </c>
-      <c r="Z6" s="5" t="n">
+      <c r="Z6" s="15" t="n">
         <v>2192470949.6515</v>
       </c>
-      <c r="AA6" s="5" t="n">
+      <c r="AA6" s="15" t="n">
         <v>2196604584.8566</v>
       </c>
-      <c r="AB6" s="5" t="n">
+      <c r="AB6" s="15" t="n">
         <v>2410132539.3328</v>
       </c>
-      <c r="AC6" s="5" t="n">
+      <c r="AC6" s="15" t="n">
         <v>2143906576.2048</v>
       </c>
-      <c r="AD6" s="5" t="n">
+      <c r="AD6" s="15" t="n">
         <v>2743455584.5329</v>
       </c>
-      <c r="AE6" s="5" t="n">
+      <c r="AE6" s="15" t="n">
         <v>2637534724.141</v>
       </c>
-      <c r="AF6" s="5" t="n">
+      <c r="AF6" s="15" t="n">
         <v>2192470949.6515</v>
       </c>
       <c r="AG6" s="7" t="n">
@@ -2450,58 +2450,58 @@
       <c r="N7" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="O7" s="5" t="n">
+      <c r="O7" s="15" t="n">
         <v>3266121388.9118</v>
       </c>
-      <c r="P7" s="5" t="n">
+      <c r="P7" s="15" t="n">
         <v>3182798416.4579</v>
       </c>
-      <c r="Q7" s="5" t="n">
+      <c r="Q7" s="15" t="n">
         <v>3233826970.6075</v>
       </c>
-      <c r="R7" s="5" t="n">
+      <c r="R7" s="15" t="n">
         <v>2767730315.3216</v>
       </c>
-      <c r="S7" s="5" t="n">
+      <c r="S7" s="15" t="n">
         <v>2660320898.8073</v>
       </c>
-      <c r="T7" s="5" t="n">
+      <c r="T7" s="15" t="n">
         <v>2350057703.0912</v>
       </c>
-      <c r="U7" s="5" t="n">
+      <c r="U7" s="15" t="n">
         <v>2090466800.5072</v>
       </c>
-      <c r="V7" s="5" t="n">
+      <c r="V7" s="15" t="n">
         <v>1852486611.2265</v>
       </c>
-      <c r="W7" s="5" t="n">
+      <c r="W7" s="15" t="n">
         <v>2095620001.2314</v>
       </c>
-      <c r="X7" s="5" t="n">
+      <c r="X7" s="15" t="n">
         <v>2157406767.1706</v>
       </c>
-      <c r="Y7" s="5" t="n">
+      <c r="Y7" s="15" t="n">
         <v>2086646758.7863</v>
       </c>
-      <c r="Z7" s="5" t="n">
+      <c r="Z7" s="15" t="n">
         <v>2954288727.5505</v>
       </c>
-      <c r="AA7" s="5" t="n">
+      <c r="AA7" s="15" t="n">
         <v>2564514717.4087</v>
       </c>
-      <c r="AB7" s="5" t="n">
+      <c r="AB7" s="15" t="n">
         <v>1728682770.7371</v>
       </c>
-      <c r="AC7" s="5" t="n">
+      <c r="AC7" s="15" t="n">
         <v>1730445562.261</v>
       </c>
-      <c r="AD7" s="5" t="n">
+      <c r="AD7" s="15" t="n">
         <v>2301474992.4097</v>
       </c>
-      <c r="AE7" s="5" t="n">
+      <c r="AE7" s="15" t="n">
         <v>2008363234.2734</v>
       </c>
-      <c r="AF7" s="5" t="n">
+      <c r="AF7" s="15" t="n">
         <v>2954288727.5505</v>
       </c>
       <c r="AG7" s="7" t="n">
@@ -2564,58 +2564,58 @@
       <c r="N8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O8" s="5" t="n">
+      <c r="O8" s="15" t="n">
         <v>16269882471.9794</v>
       </c>
-      <c r="P8" s="5" t="n">
+      <c r="P8" s="15" t="n">
         <v>17994021717.0678</v>
       </c>
-      <c r="Q8" s="5" t="n">
+      <c r="Q8" s="15" t="n">
         <v>21387199545.8055</v>
       </c>
-      <c r="R8" s="5" t="n">
+      <c r="R8" s="15" t="n">
         <v>22576338913.7346</v>
       </c>
-      <c r="S8" s="5" t="n">
+      <c r="S8" s="15" t="n">
         <v>22032636135.821</v>
       </c>
-      <c r="T8" s="5" t="n">
+      <c r="T8" s="15" t="n">
         <v>24242893687.3319</v>
       </c>
-      <c r="U8" s="5" t="n">
+      <c r="U8" s="15" t="n">
         <v>20838549418.202</v>
       </c>
-      <c r="V8" s="5" t="n">
+      <c r="V8" s="15" t="n">
         <v>24912992627.0785</v>
       </c>
-      <c r="W8" s="5" t="n">
+      <c r="W8" s="15" t="n">
         <v>22851084792.0819</v>
       </c>
-      <c r="X8" s="5" t="n">
+      <c r="X8" s="15" t="n">
         <v>24462657675.0215</v>
       </c>
-      <c r="Y8" s="5" t="n">
+      <c r="Y8" s="15" t="n">
         <v>24530048151.9762</v>
       </c>
-      <c r="Z8" s="5" t="n">
+      <c r="Z8" s="15" t="n">
         <v>30621886485.4193</v>
       </c>
-      <c r="AA8" s="5" t="n">
+      <c r="AA8" s="15" t="n">
         <v>30157803730.9944</v>
       </c>
-      <c r="AB8" s="5" t="n">
+      <c r="AB8" s="15" t="n">
         <v>34096578496.9379</v>
       </c>
-      <c r="AC8" s="5" t="n">
+      <c r="AC8" s="15" t="n">
         <v>40235083984.2429</v>
       </c>
-      <c r="AD8" s="5" t="n">
+      <c r="AD8" s="15" t="n">
         <v>37898761518.9342</v>
       </c>
-      <c r="AE8" s="5" t="n">
+      <c r="AE8" s="15" t="n">
         <v>41482341205.8373</v>
       </c>
-      <c r="AF8" s="5" t="n">
+      <c r="AF8" s="15" t="n">
         <v>30621886485.4193</v>
       </c>
       <c r="AG8" s="7" t="n">
@@ -2678,58 +2678,58 @@
       <c r="N9" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="O9" s="5" t="n">
+      <c r="O9" s="15" t="n">
         <v>295814228873.005</v>
       </c>
-      <c r="P9" s="5" t="n">
+      <c r="P9" s="15" t="n">
         <v>344228460150.258</v>
       </c>
-      <c r="Q9" s="5" t="n">
+      <c r="Q9" s="15" t="n">
         <v>331006115932.454</v>
       </c>
-      <c r="R9" s="5" t="n">
+      <c r="R9" s="15" t="n">
         <v>325466947956.52</v>
       </c>
-      <c r="S9" s="5" t="n">
+      <c r="S9" s="15" t="n">
         <v>333370444572.19</v>
       </c>
-      <c r="T9" s="5" t="n">
+      <c r="T9" s="15" t="n">
         <v>323169035400.023</v>
       </c>
-      <c r="U9" s="5" t="n">
+      <c r="U9" s="15" t="n">
         <v>275707824862.844</v>
       </c>
-      <c r="V9" s="5" t="n">
+      <c r="V9" s="15" t="n">
         <v>246953219804.49</v>
       </c>
-      <c r="W9" s="5" t="n">
+      <c r="W9" s="15" t="n">
         <v>238730914399.601</v>
       </c>
-      <c r="X9" s="5" t="n">
+      <c r="X9" s="15" t="n">
         <v>261373439540.335</v>
       </c>
-      <c r="Y9" s="5" t="n">
+      <c r="Y9" s="15" t="n">
         <v>284878416992.171</v>
       </c>
-      <c r="Z9" s="5" t="n">
+      <c r="Z9" s="15" t="n">
         <v>313701272526.863</v>
       </c>
-      <c r="AA9" s="5" t="n">
+      <c r="AA9" s="15" t="n">
         <v>339456686334.059</v>
       </c>
-      <c r="AB9" s="5" t="n">
+      <c r="AB9" s="15" t="n">
         <v>375919182099.509</v>
       </c>
-      <c r="AC9" s="5" t="n">
+      <c r="AC9" s="15" t="n">
         <v>335466315747.992</v>
       </c>
-      <c r="AD9" s="5" t="n">
+      <c r="AD9" s="15" t="n">
         <v>362818335135.692</v>
       </c>
-      <c r="AE9" s="5" t="n">
+      <c r="AE9" s="15" t="n">
         <v>400986561637.651</v>
       </c>
-      <c r="AF9" s="5" t="n">
+      <c r="AF9" s="15" t="n">
         <v>313701272526.863</v>
       </c>
       <c r="AG9" s="7" t="n">
@@ -2792,58 +2792,58 @@
       <c r="N10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="O10" s="5" t="str">
+      <c r="O10" s="15" t="str">
         <f>Sum(O2:O9)</f>
       </c>
-      <c r="P10" s="5" t="str">
+      <c r="P10" s="15" t="str">
         <f>Sum(P2:P9)</f>
       </c>
-      <c r="Q10" s="5" t="str">
+      <c r="Q10" s="15" t="str">
         <f>Sum(Q2:Q9)</f>
       </c>
-      <c r="R10" s="5" t="str">
+      <c r="R10" s="15" t="str">
         <f>Sum(R2:R9)</f>
       </c>
-      <c r="S10" s="5" t="str">
+      <c r="S10" s="15" t="str">
         <f>Sum(S2:S9)</f>
       </c>
-      <c r="T10" s="5" t="str">
+      <c r="T10" s="15" t="str">
         <f>Sum(T2:T9)</f>
       </c>
-      <c r="U10" s="5" t="str">
+      <c r="U10" s="15" t="str">
         <f>Sum(U2:U9)</f>
       </c>
-      <c r="V10" s="5" t="str">
+      <c r="V10" s="15" t="str">
         <f>Sum(V2:V9)</f>
       </c>
-      <c r="W10" s="5" t="str">
+      <c r="W10" s="15" t="str">
         <f>Sum(W2:W9)</f>
       </c>
-      <c r="X10" s="5" t="str">
+      <c r="X10" s="15" t="str">
         <f>Sum(X2:X9)</f>
       </c>
-      <c r="Y10" s="5" t="str">
+      <c r="Y10" s="15" t="str">
         <f>Sum(Y2:Y9)</f>
       </c>
-      <c r="Z10" s="5" t="str">
+      <c r="Z10" s="15" t="str">
         <f>Sum(Z2:Z9)</f>
       </c>
-      <c r="AA10" s="5" t="str">
+      <c r="AA10" s="15" t="str">
         <f>Sum(AA2:AA9)</f>
       </c>
-      <c r="AB10" s="5" t="str">
+      <c r="AB10" s="15" t="str">
         <f>Sum(AB2:AB9)</f>
       </c>
-      <c r="AC10" s="5" t="str">
+      <c r="AC10" s="15" t="str">
         <f>Sum(AC2:AC9)</f>
       </c>
-      <c r="AD10" s="5" t="str">
+      <c r="AD10" s="15" t="str">
         <f>Sum(AD2:AD9)</f>
       </c>
-      <c r="AE10" s="5" t="str">
+      <c r="AE10" s="15" t="str">
         <f>Sum(AE2:AE9)</f>
       </c>
-      <c r="AF10" s="5" t="str">
+      <c r="AF10" s="15" t="str">
         <f>Sum(AF2:AF9)</f>
       </c>
       <c r="AG10" s="7" t="str">
@@ -3374,58 +3374,58 @@
       <c r="N2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="15" t="n">
+      <c r="O2" s="9" t="n">
         <v>25125249218.822</v>
       </c>
-      <c r="P2" s="15" t="n">
+      <c r="P2" s="9" t="n">
         <v>32432154150.1501</v>
       </c>
-      <c r="Q2" s="15" t="n">
+      <c r="Q2" s="9" t="n">
         <v>35101354776.0543</v>
       </c>
-      <c r="R2" s="15" t="n">
+      <c r="R2" s="9" t="n">
         <v>30976397289.3347</v>
       </c>
-      <c r="S2" s="15" t="n">
+      <c r="S2" s="9" t="n">
         <v>31255230749.4631</v>
       </c>
-      <c r="T2" s="15" t="n">
+      <c r="T2" s="9" t="n">
         <v>37102041368.9613</v>
       </c>
-      <c r="U2" s="15" t="n">
+      <c r="U2" s="9" t="n">
         <v>24098497564.8245</v>
       </c>
-      <c r="V2" s="15" t="n">
+      <c r="V2" s="9" t="n">
         <v>19955253890.9386</v>
       </c>
-      <c r="W2" s="15" t="n">
+      <c r="W2" s="9" t="n">
         <v>17685561455.4229</v>
       </c>
-      <c r="X2" s="15" t="n">
+      <c r="X2" s="9" t="n">
         <v>16953492843.1271</v>
       </c>
-      <c r="Y2" s="15" t="n">
+      <c r="Y2" s="9" t="n">
         <v>19618603081.6569</v>
       </c>
-      <c r="Z2" s="15" t="n">
+      <c r="Z2" s="9" t="n">
         <v>27902395775.5896</v>
       </c>
-      <c r="AA2" s="15" t="n">
+      <c r="AA2" s="9" t="n">
         <v>27937731136.7199</v>
       </c>
-      <c r="AB2" s="15" t="n">
+      <c r="AB2" s="9" t="n">
         <v>30079444637.0538</v>
       </c>
-      <c r="AC2" s="15" t="n">
+      <c r="AC2" s="9" t="n">
         <v>48180087109.2192</v>
       </c>
-      <c r="AD2" s="15" t="n">
+      <c r="AD2" s="9" t="n">
         <v>45664353375.3831</v>
       </c>
-      <c r="AE2" s="15" t="n">
+      <c r="AE2" s="9" t="n">
         <v>35047872671.8265</v>
       </c>
-      <c r="AF2" s="15"/>
+      <c r="AF2" s="9"/>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -3443,58 +3443,58 @@
       <c r="N3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="O3" s="15" t="n">
+      <c r="O3" s="9" t="n">
         <v>21764778991.8306</v>
       </c>
-      <c r="P3" s="15" t="n">
+      <c r="P3" s="9" t="n">
         <v>25397309265.3422</v>
       </c>
-      <c r="Q3" s="15" t="n">
+      <c r="Q3" s="9" t="n">
         <v>21427494919.4928</v>
       </c>
-      <c r="R3" s="15" t="n">
+      <c r="R3" s="9" t="n">
         <v>18453893838.1832</v>
       </c>
-      <c r="S3" s="15" t="n">
+      <c r="S3" s="9" t="n">
         <v>17986659166.4393</v>
       </c>
-      <c r="T3" s="15" t="n">
+      <c r="T3" s="9" t="n">
         <v>16348272545.4679</v>
       </c>
-      <c r="U3" s="15" t="n">
+      <c r="U3" s="9" t="n">
         <v>13779748256.7072</v>
       </c>
-      <c r="V3" s="15" t="n">
+      <c r="V3" s="9" t="n">
         <v>11779135889.3652</v>
       </c>
-      <c r="W3" s="15" t="n">
+      <c r="W3" s="9" t="n">
         <v>12135186874.4357</v>
       </c>
-      <c r="X3" s="15" t="n">
+      <c r="X3" s="9" t="n">
         <v>12399920173.1958</v>
       </c>
-      <c r="Y3" s="15" t="n">
+      <c r="Y3" s="9" t="n">
         <v>14152861790.103</v>
       </c>
-      <c r="Z3" s="15" t="n">
+      <c r="Z3" s="9" t="n">
         <v>22806770846.0249</v>
       </c>
-      <c r="AA3" s="15" t="n">
+      <c r="AA3" s="9" t="n">
         <v>25680118499.9135</v>
       </c>
-      <c r="AB3" s="15" t="n">
+      <c r="AB3" s="9" t="n">
         <v>29875164701.4216</v>
       </c>
-      <c r="AC3" s="15" t="n">
+      <c r="AC3" s="9" t="n">
         <v>37403494926.075</v>
       </c>
-      <c r="AD3" s="15" t="n">
+      <c r="AD3" s="9" t="n">
         <v>29140563384.389</v>
       </c>
-      <c r="AE3" s="15" t="n">
+      <c r="AE3" s="9" t="n">
         <v>29077141051.9964</v>
       </c>
-      <c r="AF3" s="15"/>
+      <c r="AF3" s="9"/>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -3512,58 +3512,58 @@
       <c r="N4" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="O4" s="15" t="n">
+      <c r="O4" s="9" t="n">
         <v>30133800884.701</v>
       </c>
-      <c r="P4" s="15" t="n">
+      <c r="P4" s="9" t="n">
         <v>33783198213.0075</v>
       </c>
-      <c r="Q4" s="15" t="n">
+      <c r="Q4" s="9" t="n">
         <v>29711948309.4815</v>
       </c>
-      <c r="R4" s="15" t="n">
+      <c r="R4" s="9" t="n">
         <v>30392248649.1018</v>
       </c>
-      <c r="S4" s="15" t="n">
+      <c r="S4" s="9" t="n">
         <v>29898796158.4983</v>
       </c>
-      <c r="T4" s="15" t="n">
+      <c r="T4" s="9" t="n">
         <v>28986353557.0245</v>
       </c>
-      <c r="U4" s="15" t="n">
+      <c r="U4" s="9" t="n">
         <v>24976096489.8093</v>
       </c>
-      <c r="V4" s="15" t="n">
+      <c r="V4" s="9" t="n">
         <v>28501413952.5891</v>
       </c>
-      <c r="W4" s="15" t="n">
+      <c r="W4" s="9" t="n">
         <v>25447190127.4247</v>
       </c>
-      <c r="X4" s="15" t="n">
+      <c r="X4" s="9" t="n">
         <v>25671472541.9195</v>
       </c>
-      <c r="Y4" s="15" t="n">
+      <c r="Y4" s="9" t="n">
         <v>27983478293.0834</v>
       </c>
-      <c r="Z4" s="15" t="n">
+      <c r="Z4" s="9" t="n">
         <v>20045971011.5824</v>
       </c>
-      <c r="AA4" s="15" t="n">
+      <c r="AA4" s="9" t="n">
         <v>23936231639.1294</v>
       </c>
-      <c r="AB4" s="15" t="n">
+      <c r="AB4" s="9" t="n">
         <v>25650928177.9626</v>
       </c>
-      <c r="AC4" s="15" t="n">
+      <c r="AC4" s="9" t="n">
         <v>24016153025.3683</v>
       </c>
-      <c r="AD4" s="15" t="n">
+      <c r="AD4" s="9" t="n">
         <v>40078319954.0187</v>
       </c>
-      <c r="AE4" s="15" t="n">
+      <c r="AE4" s="9" t="n">
         <v>27163604882.0461</v>
       </c>
-      <c r="AF4" s="15"/>
+      <c r="AF4" s="9"/>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -3581,58 +3581,58 @@
       <c r="N5" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="15" t="n">
+      <c r="O5" s="9" t="n">
         <v>20416382855.5625</v>
       </c>
-      <c r="P5" s="15" t="n">
+      <c r="P5" s="9" t="n">
         <v>25609454024.9063</v>
       </c>
-      <c r="Q5" s="15" t="n">
+      <c r="Q5" s="9" t="n">
         <v>12593611119.7175</v>
       </c>
-      <c r="R5" s="15" t="n">
+      <c r="R5" s="9" t="n">
         <v>29718480733.7495</v>
       </c>
-      <c r="S5" s="15" t="n">
+      <c r="S5" s="9" t="n">
         <v>36097737150.8889</v>
       </c>
-      <c r="T5" s="15" t="n">
+      <c r="T5" s="9" t="n">
         <v>34730237706.1415</v>
       </c>
-      <c r="U5" s="15" t="n">
+      <c r="U5" s="9" t="n">
         <v>29169239953.7346</v>
       </c>
-      <c r="V5" s="15" t="n">
+      <c r="V5" s="9" t="n">
         <v>29833721322.4015</v>
       </c>
-      <c r="W5" s="15" t="n">
+      <c r="W5" s="9" t="n">
         <v>27324207449.885</v>
       </c>
-      <c r="X5" s="15" t="n">
+      <c r="X5" s="9" t="n">
         <v>27843792311.2441</v>
       </c>
-      <c r="Y5" s="15" t="n">
+      <c r="Y5" s="9" t="n">
         <v>27441082756.5163</v>
       </c>
-      <c r="Z5" s="15" t="n">
+      <c r="Z5" s="9" t="n">
         <v>23791495332.7767</v>
       </c>
-      <c r="AA5" s="15" t="n">
+      <c r="AA5" s="9" t="n">
         <v>25021165431.6188</v>
       </c>
-      <c r="AB5" s="15" t="n">
+      <c r="AB5" s="9" t="n">
         <v>27652465150.9804</v>
       </c>
-      <c r="AC5" s="15" t="n">
+      <c r="AC5" s="9" t="n">
         <v>24861742523.0282</v>
       </c>
-      <c r="AD5" s="15" t="n">
+      <c r="AD5" s="9" t="n">
         <v>29689860380.1717</v>
       </c>
-      <c r="AE5" s="15" t="n">
+      <c r="AE5" s="9" t="n">
         <v>33301971196.0154</v>
       </c>
-      <c r="AF5" s="15"/>
+      <c r="AF5" s="9"/>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -3650,58 +3650,58 @@
       <c r="N6" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="O6" s="15" t="n">
+      <c r="O6" s="9" t="n">
         <v>10096271672.9484</v>
       </c>
-      <c r="P6" s="15" t="n">
+      <c r="P6" s="9" t="n">
         <v>10776155276.9025</v>
       </c>
-      <c r="Q6" s="15" t="n">
+      <c r="Q6" s="9" t="n">
         <v>9150118544.2025</v>
       </c>
-      <c r="R6" s="15" t="n">
+      <c r="R6" s="9" t="n">
         <v>7690106134.7461</v>
       </c>
-      <c r="S6" s="15" t="n">
+      <c r="S6" s="9" t="n">
         <v>6683672074.0927</v>
       </c>
-      <c r="T6" s="15" t="n">
+      <c r="T6" s="9" t="n">
         <v>6610387564.2734</v>
       </c>
-      <c r="U6" s="15" t="n">
+      <c r="U6" s="9" t="n">
         <v>5668554306.1156</v>
       </c>
-      <c r="V6" s="15" t="n">
+      <c r="V6" s="9" t="n">
         <v>7257445382.0936</v>
       </c>
-      <c r="W6" s="15" t="n">
+      <c r="W6" s="9" t="n">
         <v>7750481635.5216</v>
       </c>
-      <c r="X6" s="15" t="n">
+      <c r="X6" s="9" t="n">
         <v>7733252678.4108</v>
       </c>
-      <c r="Y6" s="15" t="n">
+      <c r="Y6" s="9" t="n">
         <v>7150281486.2274</v>
       </c>
-      <c r="Z6" s="15" t="n">
+      <c r="Z6" s="9" t="n">
         <v>13058816162.6805</v>
       </c>
-      <c r="AA6" s="15" t="n">
+      <c r="AA6" s="9" t="n">
         <v>13269959464.3028</v>
       </c>
-      <c r="AB6" s="15" t="n">
+      <c r="AB6" s="9" t="n">
         <v>12533350568.3599</v>
       </c>
-      <c r="AC6" s="15" t="n">
+      <c r="AC6" s="9" t="n">
         <v>11545432225.8644</v>
       </c>
-      <c r="AD6" s="15" t="n">
+      <c r="AD6" s="9" t="n">
         <v>11640593258.8436</v>
       </c>
-      <c r="AE6" s="15" t="n">
+      <c r="AE6" s="9" t="n">
         <v>12484524362.2018</v>
       </c>
-      <c r="AF6" s="15"/>
+      <c r="AF6" s="9"/>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -3719,58 +3719,58 @@
       <c r="N7" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="O7" s="15" t="n">
+      <c r="O7" s="9" t="n">
         <v>10791385424.558</v>
       </c>
-      <c r="P7" s="15" t="n">
+      <c r="P7" s="9" t="n">
         <v>9992326943.864</v>
       </c>
-      <c r="Q7" s="15" t="n">
+      <c r="Q7" s="9" t="n">
         <v>10704831009.3607</v>
       </c>
-      <c r="R7" s="15" t="n">
+      <c r="R7" s="9" t="n">
         <v>10353345215.9397</v>
       </c>
-      <c r="S7" s="15" t="n">
+      <c r="S7" s="9" t="n">
         <v>14043087841.8619</v>
       </c>
-      <c r="T7" s="15" t="n">
+      <c r="T7" s="9" t="n">
         <v>12705160227.6934</v>
       </c>
-      <c r="U7" s="15" t="n">
+      <c r="U7" s="9" t="n">
         <v>10588302252.8571</v>
       </c>
-      <c r="V7" s="15" t="n">
+      <c r="V7" s="9" t="n">
         <v>10767875507.0851</v>
       </c>
-      <c r="W7" s="15" t="n">
+      <c r="W7" s="9" t="n">
         <v>10581178707.2994</v>
       </c>
-      <c r="X7" s="15" t="n">
+      <c r="X7" s="9" t="n">
         <v>9892515561.5923</v>
       </c>
-      <c r="Y7" s="15" t="n">
+      <c r="Y7" s="9" t="n">
         <v>10875001083.978</v>
       </c>
-      <c r="Z7" s="15" t="n">
+      <c r="Z7" s="9" t="n">
         <v>13483951403.3545</v>
       </c>
-      <c r="AA7" s="15" t="n">
+      <c r="AA7" s="9" t="n">
         <v>13505530020.2325</v>
       </c>
-      <c r="AB7" s="15" t="n">
+      <c r="AB7" s="9" t="n">
         <v>12588239758.5437</v>
       </c>
-      <c r="AC7" s="15" t="n">
+      <c r="AC7" s="9" t="n">
         <v>10920527227.2435</v>
       </c>
-      <c r="AD7" s="15" t="n">
+      <c r="AD7" s="9" t="n">
         <v>12179870156.4561</v>
       </c>
-      <c r="AE7" s="15" t="n">
+      <c r="AE7" s="9" t="n">
         <v>8757199136.17</v>
       </c>
-      <c r="AF7" s="15"/>
+      <c r="AF7" s="9"/>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -3788,58 +3788,58 @@
       <c r="N8" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="O8" s="15" t="n">
+      <c r="O8" s="9" t="n">
         <v>4872106.125</v>
       </c>
-      <c r="P8" s="15" t="n">
+      <c r="P8" s="9" t="n">
         <v>10010929.3706</v>
       </c>
-      <c r="Q8" s="15" t="n">
+      <c r="Q8" s="9" t="n">
         <v>16826903.2031</v>
       </c>
-      <c r="R8" s="15" t="n">
+      <c r="R8" s="9" t="n">
         <v>377038220.8154</v>
       </c>
-      <c r="S8" s="15" t="n">
+      <c r="S8" s="9" t="n">
         <v>1216030256.841</v>
       </c>
-      <c r="T8" s="15" t="n">
+      <c r="T8" s="9" t="n">
         <v>1895556032.0051</v>
       </c>
-      <c r="U8" s="15" t="n">
+      <c r="U8" s="9" t="n">
         <v>952609585.9737</v>
       </c>
-      <c r="V8" s="15" t="n">
+      <c r="V8" s="9" t="n">
         <v>1088936204.6172</v>
       </c>
-      <c r="W8" s="15" t="n">
+      <c r="W8" s="9" t="n">
         <v>1088807391.037</v>
       </c>
-      <c r="X8" s="15" t="n">
+      <c r="X8" s="9" t="n">
         <v>1805760317.0083</v>
       </c>
-      <c r="Y8" s="15" t="n">
+      <c r="Y8" s="9" t="n">
         <v>3746475883.7796</v>
       </c>
-      <c r="Z8" s="15" t="n">
+      <c r="Z8" s="9" t="n">
         <v>3074792651.2968</v>
       </c>
-      <c r="AA8" s="15" t="n">
+      <c r="AA8" s="9" t="n">
         <v>3514832423.2951</v>
       </c>
-      <c r="AB8" s="15" t="n">
+      <c r="AB8" s="9" t="n">
         <v>3566340166.6762</v>
       </c>
-      <c r="AC8" s="15" t="n">
+      <c r="AC8" s="9" t="n">
         <v>2458364985.2205</v>
       </c>
-      <c r="AD8" s="15" t="n">
+      <c r="AD8" s="9" t="n">
         <v>4576147114.9178</v>
       </c>
-      <c r="AE8" s="15" t="n">
+      <c r="AE8" s="9" t="n">
         <v>2076520940.4654</v>
       </c>
-      <c r="AF8" s="15"/>
+      <c r="AF8" s="9"/>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -3857,58 +3857,58 @@
       <c r="N9" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="O9" s="15" t="n">
+      <c r="O9" s="9" t="n">
         <v>122676909.5722</v>
       </c>
-      <c r="P9" s="15" t="n">
+      <c r="P9" s="9" t="n">
         <v>54479568.8939</v>
       </c>
-      <c r="Q9" s="15" t="n">
+      <c r="Q9" s="9" t="n">
         <v>391296344.5801</v>
       </c>
-      <c r="R9" s="15" t="n">
+      <c r="R9" s="9" t="n">
         <v>10450086106.923</v>
       </c>
-      <c r="S9" s="15" t="n">
+      <c r="S9" s="9" t="n">
         <v>42256131517.5522</v>
       </c>
-      <c r="T9" s="15" t="n">
+      <c r="T9" s="9" t="n">
         <v>54758606786.2011</v>
       </c>
-      <c r="U9" s="15" t="n">
+      <c r="U9" s="9" t="n">
         <v>46972259182.0756</v>
       </c>
-      <c r="V9" s="15" t="n">
+      <c r="V9" s="9" t="n">
         <v>43922166334.1481</v>
       </c>
-      <c r="W9" s="15" t="n">
+      <c r="W9" s="9" t="n">
         <v>44054842375.5884</v>
       </c>
-      <c r="X9" s="15" t="n">
+      <c r="X9" s="9" t="n">
         <v>50628266020.741</v>
       </c>
-      <c r="Y9" s="15" t="n">
+      <c r="Y9" s="9" t="n">
         <v>56597028392.347</v>
       </c>
-      <c r="Z9" s="15" t="n">
+      <c r="Z9" s="9" t="n">
         <v>76051318984.9463</v>
       </c>
-      <c r="AA9" s="15" t="n">
+      <c r="AA9" s="9" t="n">
         <v>80155056064.1126</v>
       </c>
-      <c r="AB9" s="15" t="n">
+      <c r="AB9" s="9" t="n">
         <v>86732963948.1466</v>
       </c>
-      <c r="AC9" s="15" t="n">
+      <c r="AC9" s="9" t="n">
         <v>85236793261.6524</v>
       </c>
-      <c r="AD9" s="15" t="n">
+      <c r="AD9" s="9" t="n">
         <v>86480545057.8842</v>
       </c>
-      <c r="AE9" s="15" t="n">
+      <c r="AE9" s="9" t="n">
         <v>59404120556.1747</v>
       </c>
-      <c r="AF9" s="15"/>
+      <c r="AF9" s="9"/>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -3926,58 +3926,58 @@
       <c r="N10" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="O10" s="15" t="n">
+      <c r="O10" s="9" t="n">
         <v>7826918502.6366</v>
       </c>
-      <c r="P10" s="15" t="n">
+      <c r="P10" s="9" t="n">
         <v>8253616344.955</v>
       </c>
-      <c r="Q10" s="15" t="n">
+      <c r="Q10" s="9" t="n">
         <v>7779611725.3281</v>
       </c>
-      <c r="R10" s="15" t="n">
+      <c r="R10" s="9" t="n">
         <v>6978787870.4494</v>
       </c>
-      <c r="S10" s="15" t="n">
+      <c r="S10" s="9" t="n">
         <v>1589089357.9102</v>
       </c>
-      <c r="T10" s="15" t="n">
+      <c r="T10" s="9" t="n">
         <v>3806242776.4534</v>
       </c>
-      <c r="U10" s="15" t="n">
+      <c r="U10" s="9" t="n">
         <v>3186009489.4102</v>
       </c>
-      <c r="V10" s="15" t="n">
+      <c r="V10" s="9" t="n">
         <v>3397043185.6465</v>
       </c>
-      <c r="W10" s="15" t="n">
+      <c r="W10" s="9" t="n">
         <v>2978381931.1913</v>
       </c>
-      <c r="X10" s="15" t="n">
+      <c r="X10" s="9" t="n">
         <v>3000039224.0025</v>
       </c>
-      <c r="Y10" s="15" t="n">
+      <c r="Y10" s="9" t="n">
         <v>2343288254.6046</v>
       </c>
-      <c r="Z10" s="15" t="n">
+      <c r="Z10" s="9" t="n">
         <v>415958942.3649</v>
       </c>
-      <c r="AA10" s="15" t="n">
+      <c r="AA10" s="9" t="n">
         <v>3483042753.0994</v>
       </c>
-      <c r="AB10" s="15" t="n">
+      <c r="AB10" s="9" t="n">
         <v>1536047657.3333</v>
       </c>
-      <c r="AC10" s="15" t="n">
+      <c r="AC10" s="9" t="n">
         <v>369757606.443</v>
       </c>
-      <c r="AD10" s="15" t="n">
+      <c r="AD10" s="9" t="n">
         <v>1101191822.3893</v>
       </c>
-      <c r="AE10" s="15" t="n">
+      <c r="AE10" s="9" t="n">
         <v>385133330.092</v>
       </c>
-      <c r="AF10" s="15"/>
+      <c r="AF10" s="9"/>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -3992,58 +3992,58 @@
       <c r="N11" t="s">
         <v>43</v>
       </c>
-      <c r="O11" s="15" t="n">
+      <c r="O11" s="9" t="n">
         <v>70636499294.0989</v>
       </c>
-      <c r="P11" s="15" t="n">
+      <c r="P11" s="9" t="n">
         <v>80526620958.9503</v>
       </c>
-      <c r="Q11" s="15" t="n">
+      <c r="Q11" s="9" t="n">
         <v>97471448187.0059</v>
       </c>
-      <c r="R11" s="15" t="n">
+      <c r="R11" s="9" t="n">
         <v>123141610571.659</v>
       </c>
-      <c r="S11" s="15" t="n">
+      <c r="S11" s="9" t="n">
         <v>115676582642.597</v>
       </c>
-      <c r="T11" s="15" t="n">
+      <c r="T11" s="9" t="n">
         <v>110877916822.175</v>
       </c>
-      <c r="U11" s="15" t="n">
+      <c r="U11" s="9" t="n">
         <v>111906304352.342</v>
       </c>
-      <c r="V11" s="15" t="n">
+      <c r="V11" s="9" t="n">
         <v>92942036400.604</v>
       </c>
-      <c r="W11" s="15" t="n">
+      <c r="W11" s="9" t="n">
         <v>93714612881.1281</v>
       </c>
-      <c r="X11" s="15" t="n">
+      <c r="X11" s="9" t="n">
         <v>112400072395.818</v>
       </c>
-      <c r="Y11" s="15" t="n">
+      <c r="Y11" s="9" t="n">
         <v>119242101605.544</v>
       </c>
-      <c r="Z11" s="15" t="n">
+      <c r="Z11" s="9" t="n">
         <v>121279137559.457</v>
       </c>
-      <c r="AA11" s="15" t="n">
+      <c r="AA11" s="9" t="n">
         <v>130516724929.479</v>
       </c>
-      <c r="AB11" s="15" t="n">
+      <c r="AB11" s="9" t="n">
         <v>154335282741.837</v>
       </c>
-      <c r="AC11" s="15" t="n">
+      <c r="AC11" s="9" t="n">
         <v>106983409731.336</v>
       </c>
-      <c r="AD11" s="15" t="n">
+      <c r="AD11" s="9" t="n">
         <v>118211663854.914</v>
       </c>
-      <c r="AE11" s="15" t="n">
+      <c r="AE11" s="9" t="n">
         <v>194346193394.303</v>
       </c>
-      <c r="AF11" s="15"/>
+      <c r="AF11" s="9"/>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -4058,58 +4058,58 @@
       <c r="N12" t="s">
         <v>40</v>
       </c>
-      <c r="O12" s="15" t="n">
+      <c r="O12" s="9" t="n">
         <v>3480708</v>
       </c>
-      <c r="P12" s="15" t="n">
+      <c r="P12" s="9" t="n">
         <v>7322732</v>
       </c>
-      <c r="Q12" s="15" t="n">
+      <c r="Q12" s="9" t="n">
         <v>4777682.7812</v>
       </c>
-      <c r="R12" s="15" t="n">
+      <c r="R12" s="9" t="n">
         <v>-389371.9688</v>
       </c>
-      <c r="S12" s="15" t="n">
+      <c r="S12" s="9" t="n">
         <v>566868.625</v>
       </c>
-      <c r="T12" s="15" t="n">
+      <c r="T12" s="9" t="n">
         <v>2744757.5625</v>
       </c>
-      <c r="U12" s="15" t="n">
+      <c r="U12" s="9" t="n">
         <v>740760.72</v>
       </c>
-      <c r="V12" s="15" t="n">
+      <c r="V12" s="9" t="n">
         <v>1661330.44</v>
       </c>
-      <c r="W12" s="15" t="n">
+      <c r="W12" s="9" t="n">
         <v>688122.1</v>
       </c>
-      <c r="X12" s="15" t="n">
+      <c r="X12" s="9" t="n">
         <v>7466648.5097</v>
       </c>
-      <c r="Y12" s="15" t="n">
+      <c r="Y12" s="9" t="n">
         <v>15539948.7242</v>
       </c>
-      <c r="Z12" s="15" t="n">
+      <c r="Z12" s="9" t="n">
         <v>10103095.4844</v>
       </c>
-      <c r="AA12" s="15" t="n">
+      <c r="AA12" s="9" t="n">
         <v>50250051.3516</v>
       </c>
-      <c r="AB12" s="15" t="n">
+      <c r="AB12" s="9" t="n">
         <v>648763.1608</v>
       </c>
-      <c r="AC12" s="15" t="n">
+      <c r="AC12" s="9" t="n">
         <v>18838219.6031</v>
       </c>
-      <c r="AD12" s="15" t="n">
+      <c r="AD12" s="9" t="n">
         <v>6404705</v>
       </c>
-      <c r="AE12" s="15" t="n">
+      <c r="AE12" s="9" t="n">
         <v>3009276.3125</v>
       </c>
-      <c r="AF12" s="15"/>
+      <c r="AF12" s="9"/>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -4151,58 +4151,58 @@
       <c r="N13" t="s">
         <v>43</v>
       </c>
-      <c r="O13" s="15" t="n">
+      <c r="O13" s="9" t="n">
         <v>91464160.72</v>
       </c>
-      <c r="P13" s="15" t="n">
+      <c r="P13" s="9" t="n">
         <v>271808916.5216</v>
       </c>
-      <c r="Q13" s="15" t="n">
+      <c r="Q13" s="9" t="n">
         <v>119963396.6512</v>
       </c>
-      <c r="R13" s="15" t="n">
+      <c r="R13" s="9" t="n">
         <v>2242431224.5039</v>
       </c>
-      <c r="S13" s="15" t="n">
+      <c r="S13" s="9" t="n">
         <v>465110922.9134</v>
       </c>
-      <c r="T13" s="15" t="n">
+      <c r="T13" s="9" t="n">
         <v>326628729.6539</v>
       </c>
-      <c r="U13" s="15" t="n">
+      <c r="U13" s="9" t="n">
         <v>205092408.93</v>
       </c>
-      <c r="V13" s="15" t="n">
+      <c r="V13" s="9" t="n">
         <v>253019515.28</v>
       </c>
-      <c r="W13" s="15" t="n">
+      <c r="W13" s="9" t="n">
         <v>124594107.6519</v>
       </c>
-      <c r="X13" s="15" t="n">
+      <c r="X13" s="9" t="n">
         <v>187804273.1566</v>
       </c>
-      <c r="Y13" s="15" t="n">
+      <c r="Y13" s="9" t="n">
         <v>125983398.2189</v>
       </c>
-      <c r="Z13" s="15" t="n">
+      <c r="Z13" s="9" t="n">
         <v>141268312.7166</v>
       </c>
-      <c r="AA13" s="15" t="n">
+      <c r="AA13" s="9" t="n">
         <v>313186482.6124</v>
       </c>
-      <c r="AB13" s="15" t="n">
+      <c r="AB13" s="9" t="n">
         <v>332401939.5916</v>
       </c>
-      <c r="AC13" s="15" t="n">
+      <c r="AC13" s="9" t="n">
         <v>298326767.0599</v>
       </c>
-      <c r="AD13" s="15" t="n">
+      <c r="AD13" s="9" t="n">
         <v>340466689.9108</v>
       </c>
-      <c r="AE13" s="15" t="n">
+      <c r="AE13" s="9" t="n">
         <v>643485539.1533</v>
       </c>
-      <c r="AF13" s="15"/>
+      <c r="AF13" s="9"/>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -4244,58 +4244,58 @@
       <c r="N14" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="O14" s="15" t="n">
+      <c r="O14" s="9" t="n">
         <v>14194339455.1302</v>
       </c>
-      <c r="P14" s="15" t="n">
+      <c r="P14" s="9" t="n">
         <v>11524936620.8855</v>
       </c>
-      <c r="Q14" s="15" t="n">
+      <c r="Q14" s="9" t="n">
         <v>8049244145.7588</v>
       </c>
-      <c r="R14" s="15" t="n">
+      <c r="R14" s="9" t="n">
         <v>5040819900.3828</v>
       </c>
-      <c r="S14" s="15" t="n">
+      <c r="S14" s="9" t="n">
         <v>3950171021.6997</v>
       </c>
-      <c r="T14" s="15" t="n">
+      <c r="T14" s="9" t="n">
         <v>3068801162.256</v>
       </c>
-      <c r="U14" s="15" t="n">
+      <c r="U14" s="9" t="n">
         <v>2429204721.8738</v>
       </c>
-      <c r="V14" s="15" t="n">
+      <c r="V14" s="9" t="n">
         <v>1781912549.4149</v>
       </c>
-      <c r="W14" s="15" t="n">
+      <c r="W14" s="9" t="n">
         <v>2952746325.5791</v>
       </c>
-      <c r="X14" s="15" t="n">
+      <c r="X14" s="9" t="n">
         <v>1881817376.9132</v>
       </c>
-      <c r="Y14" s="15" t="n">
+      <c r="Y14" s="9" t="n">
         <v>1630023794.4669</v>
       </c>
-      <c r="Z14" s="15" t="n">
+      <c r="Z14" s="9" t="n">
         <v>1558787356.0103</v>
       </c>
-      <c r="AA14" s="15" t="n">
+      <c r="AA14" s="9" t="n">
         <v>1750996158.2558</v>
       </c>
-      <c r="AB14" s="15" t="n">
+      <c r="AB14" s="9" t="n">
         <v>2067193650.8017</v>
       </c>
-      <c r="AC14" s="15" t="n">
+      <c r="AC14" s="9" t="n">
         <v>1667070626.6228</v>
       </c>
-      <c r="AD14" s="15" t="n">
+      <c r="AD14" s="9" t="n">
         <v>1955667251.6509</v>
       </c>
-      <c r="AE14" s="15" t="n">
+      <c r="AE14" s="9" t="n">
         <v>4349132039.113</v>
       </c>
-      <c r="AF14" s="15"/>
+      <c r="AF14" s="9"/>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -4337,58 +4337,58 @@
       <c r="N15" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="O15" s="15" t="n">
+      <c r="O15" s="9" t="n">
         <v>101341648420.47</v>
       </c>
-      <c r="P15" s="15" t="n">
+      <c r="P15" s="9" t="n">
         <v>117004585245.029</v>
       </c>
-      <c r="Q15" s="15" t="n">
+      <c r="Q15" s="9" t="n">
         <v>110274562226.097</v>
       </c>
-      <c r="R15" s="15" t="n">
+      <c r="R15" s="9" t="n">
         <v>72501013332.7602</v>
       </c>
-      <c r="S15" s="15" t="n">
+      <c r="S15" s="9" t="n">
         <v>51025818982.3669</v>
       </c>
-      <c r="T15" s="15" t="n">
+      <c r="T15" s="9" t="n">
         <v>31871614799.3289</v>
       </c>
-      <c r="U15" s="15" t="n">
+      <c r="U15" s="9" t="n">
         <v>18342934576.8084</v>
       </c>
-      <c r="V15" s="15" t="n">
+      <c r="V15" s="9" t="n">
         <v>15570162851.9346</v>
       </c>
-      <c r="W15" s="15" t="n">
+      <c r="W15" s="9" t="n">
         <v>11724223835.7693</v>
       </c>
-      <c r="X15" s="15" t="n">
+      <c r="X15" s="9" t="n">
         <v>10282103280.7543</v>
       </c>
-      <c r="Y15" s="15" t="n">
+      <c r="Y15" s="9" t="n">
         <v>11978672172.6364</v>
       </c>
-      <c r="Z15" s="15" t="n">
+      <c r="Z15" s="9" t="n">
         <v>11639281238.4459</v>
       </c>
-      <c r="AA15" s="15" t="n">
+      <c r="AA15" s="9" t="n">
         <v>10488589097.8683</v>
       </c>
-      <c r="AB15" s="15" t="n">
+      <c r="AB15" s="9" t="n">
         <v>12205328030.7975</v>
       </c>
-      <c r="AC15" s="15" t="n">
+      <c r="AC15" s="9" t="n">
         <v>11935398072.6335</v>
       </c>
-      <c r="AD15" s="15" t="n">
+      <c r="AD15" s="9" t="n">
         <v>11322813008.8678</v>
       </c>
-      <c r="AE15" s="15" t="n">
+      <c r="AE15" s="9" t="n">
         <v>26136114722.1225</v>
       </c>
-      <c r="AF15" s="15"/>
+      <c r="AF15" s="9"/>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -4430,58 +4430,58 @@
       <c r="N16" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="O16" s="15" t="n">
+      <c r="O16" s="9" t="n">
         <v>8491670881.2818</v>
       </c>
-      <c r="P16" s="15" t="n">
+      <c r="P16" s="9" t="n">
         <v>8687705764.4284</v>
       </c>
-      <c r="Q16" s="15" t="n">
+      <c r="Q16" s="9" t="n">
         <v>8192500498.0507</v>
       </c>
-      <c r="R16" s="15" t="n">
+      <c r="R16" s="9" t="n">
         <v>6004149560.1188</v>
       </c>
-      <c r="S16" s="15" t="n">
+      <c r="S16" s="9" t="n">
         <v>4938072295.3959</v>
       </c>
-      <c r="T16" s="15" t="n">
+      <c r="T16" s="9" t="n">
         <v>4827351746.8783</v>
       </c>
-      <c r="U16" s="15" t="n">
+      <c r="U16" s="9" t="n">
         <v>3555864463.6901</v>
       </c>
-      <c r="V16" s="15" t="n">
+      <c r="V16" s="9" t="n">
         <v>4021264457.9802</v>
       </c>
-      <c r="W16" s="15" t="n">
+      <c r="W16" s="9" t="n">
         <v>3644162020.2834</v>
       </c>
-      <c r="X16" s="15" t="n">
+      <c r="X16" s="9" t="n">
         <v>4529922466.4506</v>
       </c>
-      <c r="Y16" s="15" t="n">
+      <c r="Y16" s="9" t="n">
         <v>5463911101.9978</v>
       </c>
-      <c r="Z16" s="15" t="n">
+      <c r="Z16" s="9" t="n">
         <v>6604000036.1281</v>
       </c>
-      <c r="AA16" s="15" t="n">
+      <c r="AA16" s="9" t="n">
         <v>6973832250.8617</v>
       </c>
-      <c r="AB16" s="15" t="n">
+      <c r="AB16" s="9" t="n">
         <v>6959045290.4858</v>
       </c>
-      <c r="AC16" s="15" t="n">
+      <c r="AC16" s="9" t="n">
         <v>7137378488.2274</v>
       </c>
-      <c r="AD16" s="15" t="n">
+      <c r="AD16" s="9" t="n">
         <v>6767684566.4429</v>
       </c>
-      <c r="AE16" s="15" t="n">
+      <c r="AE16" s="9" t="n">
         <v>8611322470.3826</v>
       </c>
-      <c r="AF16" s="15"/>
+      <c r="AF16" s="9"/>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -4523,58 +4523,58 @@
       <c r="N17" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="O17" s="15" t="n">
+      <c r="O17" s="9" t="n">
         <v>11798390982.7529</v>
       </c>
-      <c r="P17" s="15" t="n">
+      <c r="P17" s="9" t="n">
         <v>11245213240.4152</v>
       </c>
-      <c r="Q17" s="15" t="n">
+      <c r="Q17" s="9" t="n">
         <v>11771340687.3015</v>
       </c>
-      <c r="R17" s="15" t="n">
+      <c r="R17" s="9" t="n">
         <v>9964056833.7781</v>
       </c>
-      <c r="S17" s="15" t="n">
+      <c r="S17" s="9" t="n">
         <v>13962135476.4921</v>
       </c>
-      <c r="T17" s="15" t="n">
+      <c r="T17" s="9" t="n">
         <v>13223323719.1346</v>
       </c>
-      <c r="U17" s="15" t="n">
+      <c r="U17" s="9" t="n">
         <v>11982732390.167</v>
       </c>
-      <c r="V17" s="15" t="n">
+      <c r="V17" s="9" t="n">
         <v>12114628991.1955</v>
       </c>
-      <c r="W17" s="15" t="n">
+      <c r="W17" s="9" t="n">
         <v>11977715880.2141</v>
       </c>
-      <c r="X17" s="15" t="n">
+      <c r="X17" s="9" t="n">
         <v>12243098979.518</v>
       </c>
-      <c r="Y17" s="15" t="n">
+      <c r="Y17" s="9" t="n">
         <v>12600972640.3082</v>
       </c>
-      <c r="Z17" s="15" t="n">
+      <c r="Z17" s="9" t="n">
         <v>15936721040.4715</v>
       </c>
-      <c r="AA17" s="15" t="n">
+      <c r="AA17" s="9" t="n">
         <v>16008560472.8886</v>
       </c>
-      <c r="AB17" s="15" t="n">
+      <c r="AB17" s="9" t="n">
         <v>15465173942.1724</v>
       </c>
-      <c r="AC17" s="15" t="n">
+      <c r="AC17" s="9" t="n">
         <v>14040430300.0082</v>
       </c>
-      <c r="AD17" s="15" t="n">
+      <c r="AD17" s="9" t="n">
         <v>14738116561.5618</v>
       </c>
-      <c r="AE17" s="15" t="n">
+      <c r="AE17" s="9" t="n">
         <v>11028697994.0188</v>
       </c>
-      <c r="AF17" s="15"/>
+      <c r="AF17" s="9"/>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -4616,58 +4616,58 @@
       <c r="N18" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="O18" s="15" t="n">
+      <c r="O18" s="9" t="n">
         <v>82129902.9873</v>
       </c>
-      <c r="P18" s="15" t="n">
+      <c r="P18" s="9" t="n">
         <v>1979157392.3166</v>
       </c>
-      <c r="Q18" s="15" t="n">
+      <c r="Q18" s="9" t="n">
         <v>1743462570.6264</v>
       </c>
-      <c r="R18" s="15" t="n">
+      <c r="R18" s="9" t="n">
         <v>1347048377.8865</v>
       </c>
-      <c r="S18" s="15" t="n">
+      <c r="S18" s="9" t="n">
         <v>1104815880.2662</v>
       </c>
-      <c r="T18" s="15" t="n">
+      <c r="T18" s="9" t="n">
         <v>567772243.9955</v>
       </c>
-      <c r="U18" s="15" t="n">
+      <c r="U18" s="9" t="n">
         <v>399938347.5108</v>
       </c>
-      <c r="V18" s="15" t="n">
+      <c r="V18" s="9" t="n">
         <v>355739285.8054</v>
       </c>
-      <c r="W18" s="15" t="n">
+      <c r="W18" s="9" t="n">
         <v>353003610.9832</v>
       </c>
-      <c r="X18" s="15" t="n">
+      <c r="X18" s="9" t="n">
         <v>471117220.9799</v>
       </c>
-      <c r="Y18" s="15" t="n">
+      <c r="Y18" s="9" t="n">
         <v>235979828.7612</v>
       </c>
-      <c r="Z18" s="15" t="n">
+      <c r="Z18" s="9" t="n">
         <v>279460783.4001</v>
       </c>
-      <c r="AA18" s="15" t="n">
+      <c r="AA18" s="9" t="n">
         <v>417457428.0022</v>
       </c>
-      <c r="AB18" s="15" t="n">
+      <c r="AB18" s="9" t="n">
         <v>283289326.9169</v>
       </c>
-      <c r="AC18" s="15" t="n">
+      <c r="AC18" s="9" t="n">
         <v>263570893.212</v>
       </c>
-      <c r="AD18" s="15" t="n">
+      <c r="AD18" s="9" t="n">
         <v>249258643.1787</v>
       </c>
-      <c r="AE18" s="15" t="n">
+      <c r="AE18" s="9" t="n">
         <v>1719360865.2598</v>
       </c>
-      <c r="AF18" s="15"/>
+      <c r="AF18" s="9"/>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -4709,58 +4709,58 @@
       <c r="N19" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="O19" s="15" t="n">
+      <c r="O19" s="9" t="n">
         <v>802067990.0419</v>
       </c>
-      <c r="P19" s="15" t="n">
+      <c r="P19" s="9" t="n">
         <v>6237580275.028</v>
       </c>
-      <c r="Q19" s="15" t="n">
+      <c r="Q19" s="9" t="n">
         <v>8972785642.9373</v>
       </c>
-      <c r="R19" s="15" t="n">
+      <c r="R19" s="9" t="n">
         <v>3034819834.017</v>
       </c>
-      <c r="S19" s="15" t="n">
+      <c r="S19" s="9" t="n">
         <v>2232747735.4338</v>
       </c>
-      <c r="T19" s="15" t="n">
+      <c r="T19" s="9" t="n">
         <v>1866909661.0176</v>
       </c>
-      <c r="U19" s="15" t="n">
+      <c r="U19" s="9" t="n">
         <v>1081245687.7024</v>
       </c>
-      <c r="V19" s="15" t="n">
+      <c r="V19" s="9" t="n">
         <v>966940317.8063</v>
       </c>
-      <c r="W19" s="15" t="n">
+      <c r="W19" s="9" t="n">
         <v>684434622.8569</v>
       </c>
-      <c r="X19" s="15" t="n">
+      <c r="X19" s="9" t="n">
         <v>650936555.8963</v>
       </c>
-      <c r="Y19" s="15" t="n">
+      <c r="Y19" s="9" t="n">
         <v>751047125.6847</v>
       </c>
-      <c r="Z19" s="15" t="n">
+      <c r="Z19" s="9" t="n">
         <v>729887740.8758</v>
       </c>
-      <c r="AA19" s="15" t="n">
+      <c r="AA19" s="9" t="n">
         <v>894924991.437</v>
       </c>
-      <c r="AB19" s="15" t="n">
+      <c r="AB19" s="9" t="n">
         <v>801886080.7621</v>
       </c>
-      <c r="AC19" s="15" t="n">
+      <c r="AC19" s="9" t="n">
         <v>386349244.0183</v>
       </c>
-      <c r="AD19" s="15" t="n">
+      <c r="AD19" s="9" t="n">
         <v>459658621.4169</v>
       </c>
-      <c r="AE19" s="15" t="n">
+      <c r="AE19" s="9" t="n">
         <v>1783365852.8155</v>
       </c>
-      <c r="AF19" s="15"/>
+      <c r="AF19" s="9"/>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -4802,58 +4802,58 @@
       <c r="N20" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="O20" s="15" t="str">
+      <c r="O20" s="9" t="str">
         <f>Sum(O2:O19)</f>
       </c>
-      <c r="P20" s="15" t="str">
+      <c r="P20" s="9" t="str">
         <f>Sum(P2:P19)</f>
       </c>
-      <c r="Q20" s="15" t="str">
+      <c r="Q20" s="9" t="str">
         <f>Sum(Q2:Q19)</f>
       </c>
-      <c r="R20" s="15" t="str">
+      <c r="R20" s="9" t="str">
         <f>Sum(R2:R19)</f>
       </c>
-      <c r="S20" s="15" t="str">
+      <c r="S20" s="9" t="str">
         <f>Sum(S2:S19)</f>
       </c>
-      <c r="T20" s="15" t="str">
+      <c r="T20" s="9" t="str">
         <f>Sum(T2:T19)</f>
       </c>
-      <c r="U20" s="15" t="str">
+      <c r="U20" s="9" t="str">
         <f>Sum(U2:U19)</f>
       </c>
-      <c r="V20" s="15" t="str">
+      <c r="V20" s="9" t="str">
         <f>Sum(V2:V19)</f>
       </c>
-      <c r="W20" s="15" t="str">
+      <c r="W20" s="9" t="str">
         <f>Sum(W2:W19)</f>
       </c>
-      <c r="X20" s="15" t="str">
+      <c r="X20" s="9" t="str">
         <f>Sum(X2:X19)</f>
       </c>
-      <c r="Y20" s="15" t="str">
+      <c r="Y20" s="9" t="str">
         <f>Sum(Y2:Y19)</f>
       </c>
-      <c r="Z20" s="15" t="str">
+      <c r="Z20" s="9" t="str">
         <f>Sum(Z2:Z19)</f>
       </c>
-      <c r="AA20" s="15" t="str">
+      <c r="AA20" s="9" t="str">
         <f>Sum(AA2:AA19)</f>
       </c>
-      <c r="AB20" s="15" t="str">
+      <c r="AB20" s="9" t="str">
         <f>Sum(AB2:AB19)</f>
       </c>
-      <c r="AC20" s="15" t="str">
+      <c r="AC20" s="9" t="str">
         <f>Sum(AC2:AC19)</f>
       </c>
-      <c r="AD20" s="15" t="str">
+      <c r="AD20" s="9" t="str">
         <f>Sum(AD2:AD19)</f>
       </c>
-      <c r="AE20" s="15" t="str">
+      <c r="AE20" s="9" t="str">
         <f>Sum(AE2:AE19)</f>
       </c>
-      <c r="AF20" s="15"/>
+      <c r="AF20" s="9"/>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -5146,16 +5146,16 @@
       <c r="B24" t="str">
         <f>N24</f>
       </c>
-      <c r="C24" s="15" t="str">
+      <c r="C24" s="9" t="str">
         <f>AB24</f>
       </c>
-      <c r="D24" s="15" t="str">
+      <c r="D24" s="9" t="str">
         <f>AD24</f>
       </c>
-      <c r="E24" s="15" t="str">
+      <c r="E24" s="9" t="str">
         <f>AE24</f>
       </c>
-      <c r="F24" s="15" t="str">
+      <c r="F24" s="9" t="str">
         <f>AF24</f>
       </c>
       <c r="G24" s="3" t="str">
@@ -5179,58 +5179,58 @@
       <c r="N24" t="s">
         <v>40</v>
       </c>
-      <c r="O24" s="15" t="n">
+      <c r="O24" s="9" t="n">
         <v>35572247423.751</v>
       </c>
-      <c r="P24" s="15" t="n">
+      <c r="P24" s="9" t="n">
         <v>44983445693.7452</v>
       </c>
-      <c r="Q24" s="15" t="n">
+      <c r="Q24" s="9" t="n">
         <v>48192805927.9893</v>
       </c>
-      <c r="R24" s="15" t="n">
+      <c r="R24" s="9" t="n">
         <v>42164237463.4606</v>
       </c>
-      <c r="S24" s="15" t="n">
+      <c r="S24" s="9" t="n">
         <v>41706668343.1184</v>
       </c>
-      <c r="T24" s="15" t="n">
+      <c r="T24" s="9" t="n">
         <v>48626220653.2593</v>
       </c>
-      <c r="U24" s="15" t="n">
+      <c r="U24" s="9" t="n">
         <v>31020811944.8711</v>
       </c>
-      <c r="V24" s="15" t="n">
+      <c r="V24" s="9" t="n">
         <v>25227193895.1278</v>
       </c>
-      <c r="W24" s="15" t="n">
+      <c r="W24" s="9" t="n">
         <v>22128705277.0359</v>
       </c>
-      <c r="X24" s="15" t="n">
+      <c r="X24" s="9" t="n">
         <v>21044466872.5407</v>
       </c>
-      <c r="Y24" s="15" t="n">
+      <c r="Y24" s="9" t="n">
         <v>23948428786.3791</v>
       </c>
-      <c r="Z24" s="15" t="n">
+      <c r="Z24" s="9" t="n">
         <v>33320734212.1306</v>
       </c>
-      <c r="AA24" s="15" t="n">
+      <c r="AA24" s="9" t="n">
         <v>32757264828.1729</v>
       </c>
-      <c r="AB24" s="15" t="n">
+      <c r="AB24" s="9" t="n">
         <v>34813670297.7214</v>
       </c>
-      <c r="AC24" s="15" t="n">
+      <c r="AC24" s="9" t="n">
         <v>53907820654.5716</v>
       </c>
-      <c r="AD24" s="15" t="n">
+      <c r="AD24" s="9" t="n">
         <v>47753342042.3351</v>
       </c>
-      <c r="AE24" s="15" t="n">
+      <c r="AE24" s="9" t="n">
         <v>35047872671.8265</v>
       </c>
-      <c r="AF24" s="15"/>
+      <c r="AF24" s="9"/>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -5239,16 +5239,16 @@
       <c r="B25" t="str">
         <f>N25</f>
       </c>
-      <c r="C25" s="15" t="str">
+      <c r="C25" s="9" t="str">
         <f>AB25</f>
       </c>
-      <c r="D25" s="15" t="str">
+      <c r="D25" s="9" t="str">
         <f>AD25</f>
       </c>
-      <c r="E25" s="15" t="str">
+      <c r="E25" s="9" t="str">
         <f>AE25</f>
       </c>
-      <c r="F25" s="15" t="str">
+      <c r="F25" s="9" t="str">
         <f>AF25</f>
       </c>
       <c r="G25" s="3" t="str">
@@ -5272,58 +5272,58 @@
       <c r="N25" t="s">
         <v>43</v>
       </c>
-      <c r="O25" s="15" t="n">
+      <c r="O25" s="9" t="n">
         <v>30814504432.484</v>
       </c>
-      <c r="P25" s="15" t="n">
+      <c r="P25" s="9" t="n">
         <v>35226105451.262</v>
       </c>
-      <c r="Q25" s="15" t="n">
+      <c r="Q25" s="9" t="n">
         <v>29419123870.4711</v>
       </c>
-      <c r="R25" s="15" t="n">
+      <c r="R25" s="9" t="n">
         <v>25118943131.1481</v>
       </c>
-      <c r="S25" s="15" t="n">
+      <c r="S25" s="9" t="n">
         <v>24001218690.9956</v>
       </c>
-      <c r="T25" s="15" t="n">
+      <c r="T25" s="9" t="n">
         <v>21426171681.2322</v>
       </c>
-      <c r="U25" s="15" t="n">
+      <c r="U25" s="9" t="n">
         <v>17737992925.4561</v>
       </c>
-      <c r="V25" s="15" t="n">
+      <c r="V25" s="9" t="n">
         <v>14891043061.7477</v>
       </c>
-      <c r="W25" s="15" t="n">
+      <c r="W25" s="9" t="n">
         <v>15183910021.9123</v>
       </c>
-      <c r="X25" s="15" t="n">
+      <c r="X25" s="9" t="n">
         <v>15392091277.0938</v>
       </c>
-      <c r="Y25" s="15" t="n">
+      <c r="Y25" s="9" t="n">
         <v>17276398390.4975</v>
       </c>
-      <c r="Z25" s="15" t="n">
+      <c r="Z25" s="9" t="n">
         <v>27235594954.2583</v>
       </c>
-      <c r="AA25" s="15" t="n">
+      <c r="AA25" s="9" t="n">
         <v>30110191783.4296</v>
       </c>
-      <c r="AB25" s="15" t="n">
+      <c r="AB25" s="9" t="n">
         <v>34577238594.4984</v>
       </c>
-      <c r="AC25" s="15" t="n">
+      <c r="AC25" s="9" t="n">
         <v>41850088227.4911</v>
       </c>
-      <c r="AD25" s="15" t="n">
+      <c r="AD25" s="9" t="n">
         <v>30473644927.4072</v>
       </c>
-      <c r="AE25" s="15" t="n">
+      <c r="AE25" s="9" t="n">
         <v>29077141051.9964</v>
       </c>
-      <c r="AF25" s="15"/>
+      <c r="AF25" s="9"/>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -5332,16 +5332,16 @@
       <c r="B26" t="str">
         <f>N26</f>
       </c>
-      <c r="C26" s="15" t="str">
+      <c r="C26" s="9" t="str">
         <f>AB26</f>
       </c>
-      <c r="D26" s="15" t="str">
+      <c r="D26" s="9" t="str">
         <f>AD26</f>
       </c>
-      <c r="E26" s="15" t="str">
+      <c r="E26" s="9" t="str">
         <f>AE26</f>
       </c>
-      <c r="F26" s="15" t="str">
+      <c r="F26" s="9" t="str">
         <f>AF26</f>
       </c>
       <c r="G26" s="3" t="str">
@@ -5365,58 +5365,58 @@
       <c r="N26" t="s">
         <v>40</v>
       </c>
-      <c r="O26" s="15" t="n">
+      <c r="O26" s="9" t="n">
         <v>42663338841.058</v>
       </c>
-      <c r="P26" s="15" t="n">
+      <c r="P26" s="9" t="n">
         <v>46857345803.8037</v>
       </c>
-      <c r="Q26" s="15" t="n">
+      <c r="Q26" s="9" t="n">
         <v>40793358767.9674</v>
       </c>
-      <c r="R26" s="15" t="n">
+      <c r="R26" s="9" t="n">
         <v>41369110071.7669</v>
       </c>
-      <c r="S26" s="15" t="n">
+      <c r="S26" s="9" t="n">
         <v>39896655546.6051</v>
       </c>
-      <c r="T26" s="15" t="n">
+      <c r="T26" s="9" t="n">
         <v>37989737814.7073</v>
       </c>
-      <c r="U26" s="15" t="n">
+      <c r="U26" s="9" t="n">
         <v>32150501924.163</v>
       </c>
-      <c r="V26" s="15" t="n">
+      <c r="V26" s="9" t="n">
         <v>36031147486.1144</v>
       </c>
-      <c r="W26" s="15" t="n">
+      <c r="W26" s="9" t="n">
         <v>31840288015.6125</v>
       </c>
-      <c r="X26" s="15" t="n">
+      <c r="X26" s="9" t="n">
         <v>31866144544.7672</v>
       </c>
-      <c r="Y26" s="15" t="n">
+      <c r="Y26" s="9" t="n">
         <v>34159431958.9289</v>
       </c>
-      <c r="Z26" s="15" t="n">
+      <c r="Z26" s="9" t="n">
         <v>23938678150.5467</v>
       </c>
-      <c r="AA26" s="15" t="n">
+      <c r="AA26" s="9" t="n">
         <v>28065467269.1331</v>
       </c>
-      <c r="AB26" s="15" t="n">
+      <c r="AB26" s="9" t="n">
         <v>29688146413.3836</v>
       </c>
-      <c r="AC26" s="15" t="n">
+      <c r="AC26" s="9" t="n">
         <v>26871235561.8919</v>
       </c>
-      <c r="AD26" s="15" t="n">
+      <c r="AD26" s="9" t="n">
         <v>41911766613.9588</v>
       </c>
-      <c r="AE26" s="15" t="n">
+      <c r="AE26" s="9" t="n">
         <v>27163604882.0461</v>
       </c>
-      <c r="AF26" s="15"/>
+      <c r="AF26" s="9"/>
     </row>
     <row r="27">
       <c r="A27" t="str">
@@ -5425,16 +5425,16 @@
       <c r="B27" t="str">
         <f>N27</f>
       </c>
-      <c r="C27" s="15" t="str">
+      <c r="C27" s="9" t="str">
         <f>AB27</f>
       </c>
-      <c r="D27" s="15" t="str">
+      <c r="D27" s="9" t="str">
         <f>AD27</f>
       </c>
-      <c r="E27" s="15" t="str">
+      <c r="E27" s="9" t="str">
         <f>AE27</f>
       </c>
-      <c r="F27" s="15" t="str">
+      <c r="F27" s="9" t="str">
         <f>AF27</f>
       </c>
       <c r="G27" s="3" t="str">
@@ -5458,58 +5458,58 @@
       <c r="N27" t="s">
         <v>43</v>
       </c>
-      <c r="O27" s="15" t="n">
+      <c r="O27" s="9" t="n">
         <v>28905449498.6676</v>
       </c>
-      <c r="P27" s="15" t="n">
+      <c r="P27" s="9" t="n">
         <v>35520350546.0184</v>
       </c>
-      <c r="Q27" s="15" t="n">
+      <c r="Q27" s="9" t="n">
         <v>17290542216.8818</v>
       </c>
-      <c r="R27" s="15" t="n">
+      <c r="R27" s="9" t="n">
         <v>40451995337.1894</v>
       </c>
-      <c r="S27" s="15" t="n">
+      <c r="S27" s="9" t="n">
         <v>48168460612.4704</v>
       </c>
-      <c r="T27" s="15" t="n">
+      <c r="T27" s="9" t="n">
         <v>45517716538.6861</v>
       </c>
-      <c r="U27" s="15" t="n">
+      <c r="U27" s="9" t="n">
         <v>37548129494.197</v>
       </c>
-      <c r="V27" s="15" t="n">
+      <c r="V27" s="9" t="n">
         <v>37715434568.0957</v>
       </c>
-      <c r="W27" s="15" t="n">
+      <c r="W27" s="9" t="n">
         <v>34188868423.043</v>
       </c>
-      <c r="X27" s="15" t="n">
+      <c r="X27" s="9" t="n">
         <v>34562657401.7416</v>
       </c>
-      <c r="Y27" s="15" t="n">
+      <c r="Y27" s="9" t="n">
         <v>33497329727.3143</v>
       </c>
-      <c r="Z27" s="15" t="n">
+      <c r="Z27" s="9" t="n">
         <v>28411542108.0127</v>
       </c>
-      <c r="AA27" s="15" t="n">
+      <c r="AA27" s="9" t="n">
         <v>29337562822.909</v>
       </c>
-      <c r="AB27" s="15" t="n">
+      <c r="AB27" s="9" t="n">
         <v>32004706745.8009</v>
       </c>
-      <c r="AC27" s="15" t="n">
+      <c r="AC27" s="9" t="n">
         <v>27817350227.1458</v>
       </c>
-      <c r="AD27" s="15" t="n">
+      <c r="AD27" s="9" t="n">
         <v>31048070390.2362</v>
       </c>
-      <c r="AE27" s="15" t="n">
+      <c r="AE27" s="9" t="n">
         <v>33301971196.0154</v>
       </c>
-      <c r="AF27" s="15"/>
+      <c r="AF27" s="9"/>
     </row>
     <row r="28">
       <c r="A28" t="str">
@@ -5518,16 +5518,16 @@
       <c r="B28" t="str">
         <f>N28</f>
       </c>
-      <c r="C28" s="15" t="str">
+      <c r="C28" s="9" t="str">
         <f>AB28</f>
       </c>
-      <c r="D28" s="15" t="str">
+      <c r="D28" s="9" t="str">
         <f>AD28</f>
       </c>
-      <c r="E28" s="15" t="str">
+      <c r="E28" s="9" t="str">
         <f>AE28</f>
       </c>
-      <c r="F28" s="15" t="str">
+      <c r="F28" s="9" t="str">
         <f>AF28</f>
       </c>
       <c r="G28" s="3" t="str">
@@ -5551,58 +5551,58 @@
       <c r="N28" t="s">
         <v>40</v>
       </c>
-      <c r="O28" s="15" t="n">
+      <c r="O28" s="9" t="n">
         <v>14294269118.6714</v>
       </c>
-      <c r="P28" s="15" t="n">
+      <c r="P28" s="9" t="n">
         <v>14946543280.526</v>
       </c>
-      <c r="Q28" s="15" t="n">
+      <c r="Q28" s="9" t="n">
         <v>12562759757.6282</v>
       </c>
-      <c r="R28" s="15" t="n">
+      <c r="R28" s="9" t="n">
         <v>10467565293.5369</v>
       </c>
-      <c r="S28" s="15" t="n">
+      <c r="S28" s="9" t="n">
         <v>8918625389.22816</v>
       </c>
-      <c r="T28" s="15" t="n">
+      <c r="T28" s="9" t="n">
         <v>8663624761.43503</v>
       </c>
-      <c r="U28" s="15" t="n">
+      <c r="U28" s="9" t="n">
         <v>7296851459.56864</v>
       </c>
-      <c r="V28" s="15" t="n">
+      <c r="V28" s="9" t="n">
         <v>9174775867.94883</v>
       </c>
-      <c r="W28" s="15" t="n">
+      <c r="W28" s="9" t="n">
         <v>9697635231.98454</v>
       </c>
-      <c r="X28" s="15" t="n">
+      <c r="X28" s="9" t="n">
         <v>9599330433.77419</v>
       </c>
-      <c r="Y28" s="15" t="n">
+      <c r="Y28" s="9" t="n">
         <v>8728348611.9145</v>
       </c>
-      <c r="Z28" s="15" t="n">
+      <c r="Z28" s="9" t="n">
         <v>15594694662.8298</v>
       </c>
-      <c r="AA28" s="15" t="n">
+      <c r="AA28" s="9" t="n">
         <v>15559158125.7633</v>
       </c>
-      <c r="AB28" s="15" t="n">
+      <c r="AB28" s="9" t="n">
         <v>14505983726.6789</v>
       </c>
-      <c r="AC28" s="15" t="n">
+      <c r="AC28" s="9" t="n">
         <v>12917973527.1237</v>
       </c>
-      <c r="AD28" s="15" t="n">
+      <c r="AD28" s="9" t="n">
         <v>12173110760.9404</v>
       </c>
-      <c r="AE28" s="15" t="n">
+      <c r="AE28" s="9" t="n">
         <v>12484524362.2018</v>
       </c>
-      <c r="AF28" s="15"/>
+      <c r="AF28" s="9"/>
     </row>
     <row r="29">
       <c r="A29" t="str">
@@ -5611,16 +5611,16 @@
       <c r="B29" t="str">
         <f>N29</f>
       </c>
-      <c r="C29" s="15" t="str">
+      <c r="C29" s="9" t="str">
         <f>AB29</f>
       </c>
-      <c r="D29" s="15" t="str">
+      <c r="D29" s="9" t="str">
         <f>AD29</f>
       </c>
-      <c r="E29" s="15" t="str">
+      <c r="E29" s="9" t="str">
         <f>AE29</f>
       </c>
-      <c r="F29" s="15" t="str">
+      <c r="F29" s="9" t="str">
         <f>AF29</f>
       </c>
       <c r="G29" s="3" t="str">
@@ -5644,58 +5644,58 @@
       <c r="N29" t="s">
         <v>43</v>
       </c>
-      <c r="O29" s="15" t="n">
+      <c r="O29" s="9" t="n">
         <v>15278408943.2979</v>
       </c>
-      <c r="P29" s="15" t="n">
+      <c r="P29" s="9" t="n">
         <v>13859372225.2449</v>
       </c>
-      <c r="Q29" s="15" t="n">
+      <c r="Q29" s="9" t="n">
         <v>14697319992.8448</v>
       </c>
-      <c r="R29" s="15" t="n">
+      <c r="R29" s="9" t="n">
         <v>14092694581.2504</v>
       </c>
-      <c r="S29" s="15" t="n">
+      <c r="S29" s="9" t="n">
         <v>18738956427.1213</v>
       </c>
-      <c r="T29" s="15" t="n">
+      <c r="T29" s="9" t="n">
         <v>16651480669.8392</v>
       </c>
-      <c r="U29" s="15" t="n">
+      <c r="U29" s="9" t="n">
         <v>13629801281.9177</v>
       </c>
-      <c r="V29" s="15" t="n">
+      <c r="V29" s="9" t="n">
         <v>13612619751.1916</v>
       </c>
-      <c r="W29" s="15" t="n">
+      <c r="W29" s="9" t="n">
         <v>13239488363.8642</v>
       </c>
-      <c r="X29" s="15" t="n">
+      <c r="X29" s="9" t="n">
         <v>12279635703.885</v>
       </c>
-      <c r="Y29" s="15" t="n">
+      <c r="Y29" s="9" t="n">
         <v>13275113825.7621</v>
       </c>
-      <c r="Z29" s="15" t="n">
+      <c r="Z29" s="9" t="n">
         <v>16102386492.3286</v>
       </c>
-      <c r="AA29" s="15" t="n">
+      <c r="AA29" s="9" t="n">
         <v>15835366921.9804</v>
       </c>
-      <c r="AB29" s="15" t="n">
+      <c r="AB29" s="9" t="n">
         <v>14569511966.4128</v>
       </c>
-      <c r="AC29" s="15" t="n">
+      <c r="AC29" s="9" t="n">
         <v>12218778722.5267</v>
       </c>
-      <c r="AD29" s="15" t="n">
+      <c r="AD29" s="9" t="n">
         <v>12737057740.2291</v>
       </c>
-      <c r="AE29" s="15" t="n">
+      <c r="AE29" s="9" t="n">
         <v>8757199136.17</v>
       </c>
-      <c r="AF29" s="15"/>
+      <c r="AF29" s="9"/>
     </row>
     <row r="30">
       <c r="A30" t="str">
@@ -5704,16 +5704,16 @@
       <c r="B30" t="str">
         <f>N30</f>
       </c>
-      <c r="C30" s="15" t="str">
+      <c r="C30" s="9" t="str">
         <f>AB30</f>
       </c>
-      <c r="D30" s="15" t="str">
+      <c r="D30" s="9" t="str">
         <f>AD30</f>
       </c>
-      <c r="E30" s="15" t="str">
+      <c r="E30" s="9" t="str">
         <f>AE30</f>
       </c>
-      <c r="F30" s="15" t="str">
+      <c r="F30" s="9" t="str">
         <f>AF30</f>
       </c>
       <c r="G30" s="3" t="str">
@@ -5737,58 +5737,58 @@
       <c r="N30" t="s">
         <v>40</v>
       </c>
-      <c r="O30" s="15" t="n">
+      <c r="O30" s="9" t="n">
         <v>6897912.25726192</v>
       </c>
-      <c r="P30" s="15" t="n">
+      <c r="P30" s="9" t="n">
         <v>13885173.8185951</v>
       </c>
-      <c r="Q30" s="15" t="n">
+      <c r="Q30" s="9" t="n">
         <v>23102688.930664</v>
       </c>
-      <c r="R30" s="15" t="n">
+      <c r="R30" s="9" t="n">
         <v>513214268.488699</v>
       </c>
-      <c r="S30" s="15" t="n">
+      <c r="S30" s="9" t="n">
         <v>1622658652.68443</v>
       </c>
-      <c r="T30" s="15" t="n">
+      <c r="T30" s="9" t="n">
         <v>2484330308.30501</v>
       </c>
-      <c r="U30" s="15" t="n">
+      <c r="U30" s="9" t="n">
         <v>1226247517.87454</v>
       </c>
-      <c r="V30" s="15" t="n">
+      <c r="V30" s="9" t="n">
         <v>1376620158.45245</v>
       </c>
-      <c r="W30" s="15" t="n">
+      <c r="W30" s="9" t="n">
         <v>1362348485.25707</v>
       </c>
-      <c r="X30" s="15" t="n">
+      <c r="X30" s="9" t="n">
         <v>2241500528.69108</v>
       </c>
-      <c r="Y30" s="15" t="n">
+      <c r="Y30" s="9" t="n">
         <v>4573323112.20829</v>
       </c>
-      <c r="Z30" s="15" t="n">
+      <c r="Z30" s="9" t="n">
         <v>3671883572.8402</v>
       </c>
-      <c r="AA30" s="15" t="n">
+      <c r="AA30" s="9" t="n">
         <v>4121175622.78338</v>
       </c>
-      <c r="AB30" s="15" t="n">
+      <c r="AB30" s="9" t="n">
         <v>4127649038.41478</v>
       </c>
-      <c r="AC30" s="15" t="n">
+      <c r="AC30" s="9" t="n">
         <v>2750619741.02132</v>
       </c>
-      <c r="AD30" s="15" t="n">
+      <c r="AD30" s="9" t="n">
         <v>4785490262.35678</v>
       </c>
-      <c r="AE30" s="15" t="n">
+      <c r="AE30" s="9" t="n">
         <v>2076520940.4654</v>
       </c>
-      <c r="AF30" s="15"/>
+      <c r="AF30" s="9"/>
     </row>
     <row r="31">
       <c r="A31" t="str">
@@ -5797,16 +5797,16 @@
       <c r="B31" t="str">
         <f>N31</f>
       </c>
-      <c r="C31" s="15" t="str">
+      <c r="C31" s="9" t="str">
         <f>AB31</f>
       </c>
-      <c r="D31" s="15" t="str">
+      <c r="D31" s="9" t="str">
         <f>AD31</f>
       </c>
-      <c r="E31" s="15" t="str">
+      <c r="E31" s="9" t="str">
         <f>AE31</f>
       </c>
-      <c r="F31" s="15" t="str">
+      <c r="F31" s="9" t="str">
         <f>AF31</f>
       </c>
       <c r="G31" s="3" t="str">
@@ -5830,58 +5830,58 @@
       <c r="N31" t="s">
         <v>43</v>
       </c>
-      <c r="O31" s="15" t="n">
+      <c r="O31" s="9" t="n">
         <v>173685575.911196</v>
       </c>
-      <c r="P31" s="15" t="n">
+      <c r="P31" s="9" t="n">
         <v>75563242.4972936</v>
       </c>
-      <c r="Q31" s="15" t="n">
+      <c r="Q31" s="9" t="n">
         <v>537234785.238114</v>
       </c>
-      <c r="R31" s="15" t="n">
+      <c r="R31" s="9" t="n">
         <v>14224375675.7865</v>
       </c>
-      <c r="S31" s="15" t="n">
+      <c r="S31" s="9" t="n">
         <v>56386160665.1557</v>
       </c>
-      <c r="T31" s="15" t="n">
+      <c r="T31" s="9" t="n">
         <v>71767051030.2011</v>
       </c>
-      <c r="U31" s="15" t="n">
+      <c r="U31" s="9" t="n">
         <v>60465081476.2742</v>
       </c>
-      <c r="V31" s="15" t="n">
+      <c r="V31" s="9" t="n">
         <v>55525878671.4186</v>
       </c>
-      <c r="W31" s="15" t="n">
+      <c r="W31" s="9" t="n">
         <v>55122740966.5721</v>
       </c>
-      <c r="X31" s="15" t="n">
+      <c r="X31" s="9" t="n">
         <v>62845153912.9054</v>
       </c>
-      <c r="Y31" s="15" t="n">
+      <c r="Y31" s="9" t="n">
         <v>69087992571.8098</v>
       </c>
-      <c r="Z31" s="15" t="n">
+      <c r="Z31" s="9" t="n">
         <v>90819648848.8026</v>
       </c>
-      <c r="AA31" s="15" t="n">
+      <c r="AA31" s="9" t="n">
         <v>93982592428.8516</v>
       </c>
-      <c r="AB31" s="15" t="n">
+      <c r="AB31" s="9" t="n">
         <v>100383928203.093</v>
       </c>
-      <c r="AC31" s="15" t="n">
+      <c r="AC31" s="9" t="n">
         <v>95369893248.7136</v>
       </c>
-      <c r="AD31" s="15" t="n">
+      <c r="AD31" s="9" t="n">
         <v>90436735503.6936</v>
       </c>
-      <c r="AE31" s="15" t="n">
+      <c r="AE31" s="9" t="n">
         <v>59404120556.1747</v>
       </c>
-      <c r="AF31" s="15"/>
+      <c r="AF31" s="9"/>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -5890,16 +5890,16 @@
       <c r="B32" t="str">
         <f>N32</f>
       </c>
-      <c r="C32" s="15" t="str">
+      <c r="C32" s="9" t="str">
         <f>AB32</f>
       </c>
-      <c r="D32" s="15" t="str">
+      <c r="D32" s="9" t="str">
         <f>AD32</f>
       </c>
-      <c r="E32" s="15" t="str">
+      <c r="E32" s="9" t="str">
         <f>AE32</f>
       </c>
-      <c r="F32" s="15" t="str">
+      <c r="F32" s="9" t="str">
         <f>AF32</f>
       </c>
       <c r="G32" s="3" t="str">
@@ -5923,58 +5923,58 @@
       <c r="N32" t="s">
         <v>40</v>
       </c>
-      <c r="O32" s="15" t="n">
+      <c r="O32" s="9" t="n">
         <v>11081326163.8317</v>
       </c>
-      <c r="P32" s="15" t="n">
+      <c r="P32" s="9" t="n">
         <v>11447778057.2763</v>
       </c>
-      <c r="Q32" s="15" t="n">
+      <c r="Q32" s="9" t="n">
         <v>10681106768.2668</v>
       </c>
-      <c r="R32" s="15" t="n">
+      <c r="R32" s="9" t="n">
         <v>9499338035.61011</v>
       </c>
-      <c r="S32" s="15" t="n">
+      <c r="S32" s="9" t="n">
         <v>2120464998.29722</v>
       </c>
-      <c r="T32" s="15" t="n">
+      <c r="T32" s="9" t="n">
         <v>4988491044.66079</v>
       </c>
-      <c r="U32" s="15" t="n">
+      <c r="U32" s="9" t="n">
         <v>4101193485.59845</v>
       </c>
-      <c r="V32" s="15" t="n">
+      <c r="V32" s="9" t="n">
         <v>4294501467.2723</v>
       </c>
-      <c r="W32" s="15" t="n">
+      <c r="W32" s="9" t="n">
         <v>3726640860.33707</v>
       </c>
-      <c r="X32" s="15" t="n">
+      <c r="X32" s="9" t="n">
         <v>3723965713.14435</v>
       </c>
-      <c r="Y32" s="15" t="n">
+      <c r="Y32" s="9" t="n">
         <v>2860451972.94533</v>
       </c>
-      <c r="Z32" s="15" t="n">
+      <c r="Z32" s="9" t="n">
         <v>496733594.963386</v>
       </c>
-      <c r="AA32" s="15" t="n">
+      <c r="AA32" s="9" t="n">
         <v>4083901921.48299</v>
       </c>
-      <c r="AB32" s="15" t="n">
+      <c r="AB32" s="9" t="n">
         <v>1777807314.90349</v>
       </c>
-      <c r="AC32" s="15" t="n">
+      <c r="AC32" s="9" t="n">
         <v>413715041.415498</v>
       </c>
-      <c r="AD32" s="15" t="n">
+      <c r="AD32" s="9" t="n">
         <v>1151567598.39561</v>
       </c>
-      <c r="AE32" s="15" t="n">
+      <c r="AE32" s="9" t="n">
         <v>385133330.092</v>
       </c>
-      <c r="AF32" s="15"/>
+      <c r="AF32" s="9"/>
     </row>
     <row r="33">
       <c r="A33" t="str">
@@ -5983,16 +5983,16 @@
       <c r="B33" t="str">
         <f>N33</f>
       </c>
-      <c r="C33" s="15" t="str">
+      <c r="C33" s="9" t="str">
         <f>AB33</f>
       </c>
-      <c r="D33" s="15" t="str">
+      <c r="D33" s="9" t="str">
         <f>AD33</f>
       </c>
-      <c r="E33" s="15" t="str">
+      <c r="E33" s="9" t="str">
         <f>AE33</f>
       </c>
-      <c r="F33" s="15" t="str">
+      <c r="F33" s="9" t="str">
         <f>AF33</f>
       </c>
       <c r="G33" s="3" t="str">
@@ -6016,58 +6016,58 @@
       <c r="N33" t="s">
         <v>43</v>
       </c>
-      <c r="O33" s="15" t="n">
+      <c r="O33" s="9" t="n">
         <v>100006929609.079</v>
       </c>
-      <c r="P33" s="15" t="n">
+      <c r="P33" s="9" t="n">
         <v>111690542171.124</v>
       </c>
-      <c r="Q33" s="15" t="n">
+      <c r="Q33" s="9" t="n">
         <v>133824537997.632</v>
       </c>
-      <c r="R33" s="15" t="n">
+      <c r="R33" s="9" t="n">
         <v>167617042785.157</v>
       </c>
-      <c r="S33" s="15" t="n">
+      <c r="S33" s="9" t="n">
         <v>154357678751.836</v>
       </c>
-      <c r="T33" s="15" t="n">
+      <c r="T33" s="9" t="n">
         <v>145317450200.443</v>
       </c>
-      <c r="U33" s="15" t="n">
+      <c r="U33" s="9" t="n">
         <v>144051487584.297</v>
       </c>
-      <c r="V33" s="15" t="n">
+      <c r="V33" s="9" t="n">
         <v>117496213583.669</v>
       </c>
-      <c r="W33" s="15" t="n">
+      <c r="W33" s="9" t="n">
         <v>117258536226.008</v>
       </c>
-      <c r="X33" s="15" t="n">
+      <c r="X33" s="9" t="n">
         <v>139522847704.147</v>
       </c>
-      <c r="Y33" s="15" t="n">
+      <c r="Y33" s="9" t="n">
         <v>145558833457.85</v>
       </c>
-      <c r="Z33" s="15" t="n">
+      <c r="Z33" s="9" t="n">
         <v>144830212451.88</v>
       </c>
-      <c r="AA33" s="15" t="n">
+      <c r="AA33" s="9" t="n">
         <v>153032145026.315</v>
       </c>
-      <c r="AB33" s="15" t="n">
+      <c r="AB33" s="9" t="n">
         <v>178626225101.947</v>
       </c>
-      <c r="AC33" s="15" t="n">
+      <c r="AC33" s="9" t="n">
         <v>119701785755.133</v>
       </c>
-      <c r="AD33" s="15" t="n">
+      <c r="AD33" s="9" t="n">
         <v>123619444932.3</v>
       </c>
-      <c r="AE33" s="15" t="n">
+      <c r="AE33" s="9" t="n">
         <v>194346193394.303</v>
       </c>
-      <c r="AF33" s="15"/>
+      <c r="AF33" s="9"/>
     </row>
     <row r="34">
       <c r="A34" t="str">
@@ -6076,16 +6076,16 @@
       <c r="B34" t="str">
         <f>N34</f>
       </c>
-      <c r="C34" s="15" t="str">
+      <c r="C34" s="9" t="str">
         <f>AB34</f>
       </c>
-      <c r="D34" s="15" t="str">
+      <c r="D34" s="9" t="str">
         <f>AD34</f>
       </c>
-      <c r="E34" s="15" t="str">
+      <c r="E34" s="9" t="str">
         <f>AE34</f>
       </c>
-      <c r="F34" s="15" t="str">
+      <c r="F34" s="9" t="str">
         <f>AF34</f>
       </c>
       <c r="G34" s="3" t="str">
@@ -6109,58 +6109,58 @@
       <c r="N34" t="s">
         <v>40</v>
       </c>
-      <c r="O34" s="15" t="n">
+      <c r="O34" s="9" t="n">
         <v>4927975.24543857</v>
       </c>
-      <c r="P34" s="15" t="n">
+      <c r="P34" s="9" t="n">
         <v>10156640.0963325</v>
       </c>
-      <c r="Q34" s="15" t="n">
+      <c r="Q34" s="9" t="n">
         <v>6559574.13976913</v>
       </c>
-      <c r="R34" s="15" t="n">
+      <c r="R34" s="9" t="n">
         <v>-530002.633965152</v>
       </c>
-      <c r="S34" s="15" t="n">
+      <c r="S34" s="9" t="n">
         <v>756423.842348394</v>
       </c>
-      <c r="T34" s="15" t="n">
+      <c r="T34" s="9" t="n">
         <v>3597300.3627095</v>
       </c>
-      <c r="U34" s="15" t="n">
+      <c r="U34" s="9" t="n">
         <v>953544.880939329</v>
       </c>
-      <c r="V34" s="15" t="n">
+      <c r="V34" s="9" t="n">
         <v>2100234.12194165</v>
       </c>
-      <c r="W34" s="15" t="n">
+      <c r="W34" s="9" t="n">
         <v>860999.023632689</v>
       </c>
-      <c r="X34" s="15" t="n">
+      <c r="X34" s="9" t="n">
         <v>9268393.16624881</v>
       </c>
-      <c r="Y34" s="15" t="n">
+      <c r="Y34" s="9" t="n">
         <v>18969615.411275</v>
       </c>
-      <c r="Z34" s="15" t="n">
+      <c r="Z34" s="9" t="n">
         <v>12065005.5308147</v>
       </c>
-      <c r="AA34" s="15" t="n">
+      <c r="AA34" s="9" t="n">
         <v>58918679.9636052</v>
       </c>
-      <c r="AB34" s="15" t="n">
+      <c r="AB34" s="9" t="n">
         <v>750872.466361167</v>
       </c>
-      <c r="AC34" s="15" t="n">
+      <c r="AC34" s="9" t="n">
         <v>21077740.3019894</v>
       </c>
-      <c r="AD34" s="15" t="n">
+      <c r="AD34" s="9" t="n">
         <v>6697698.44392739</v>
       </c>
-      <c r="AE34" s="15" t="n">
+      <c r="AE34" s="9" t="n">
         <v>3009276.3125</v>
       </c>
-      <c r="AF34" s="15"/>
+      <c r="AF34" s="9"/>
     </row>
     <row r="35">
       <c r="A35" t="str">
@@ -6169,16 +6169,16 @@
       <c r="B35" t="str">
         <f>N35</f>
       </c>
-      <c r="C35" s="15" t="str">
+      <c r="C35" s="9" t="str">
         <f>AB35</f>
       </c>
-      <c r="D35" s="15" t="str">
+      <c r="D35" s="9" t="str">
         <f>AD35</f>
       </c>
-      <c r="E35" s="15" t="str">
+      <c r="E35" s="9" t="str">
         <f>AE35</f>
       </c>
-      <c r="F35" s="15" t="str">
+      <c r="F35" s="9" t="str">
         <f>AF35</f>
       </c>
       <c r="G35" s="3" t="str">
@@ -6202,58 +6202,58 @@
       <c r="N35" t="s">
         <v>43</v>
       </c>
-      <c r="O35" s="15" t="n">
+      <c r="O35" s="9" t="n">
         <v>129494665.991222</v>
       </c>
-      <c r="P35" s="15" t="n">
+      <c r="P35" s="9" t="n">
         <v>376999368.553153</v>
       </c>
-      <c r="Q35" s="15" t="n">
+      <c r="Q35" s="9" t="n">
         <v>164705115.519292</v>
       </c>
-      <c r="R35" s="15" t="n">
+      <c r="R35" s="9" t="n">
         <v>3052336970.05866</v>
       </c>
-      <c r="S35" s="15" t="n">
+      <c r="S35" s="9" t="n">
         <v>620639379.059586</v>
       </c>
-      <c r="T35" s="15" t="n">
+      <c r="T35" s="9" t="n">
         <v>428082124.158577</v>
       </c>
-      <c r="U35" s="15" t="n">
+      <c r="U35" s="9" t="n">
         <v>264005381.730712</v>
       </c>
-      <c r="V35" s="15" t="n">
+      <c r="V35" s="9" t="n">
         <v>319864252.59757</v>
       </c>
-      <c r="W35" s="15" t="n">
+      <c r="W35" s="9" t="n">
         <v>155895886.847221</v>
       </c>
-      <c r="X35" s="15" t="n">
+      <c r="X35" s="9" t="n">
         <v>233122510.00642</v>
       </c>
-      <c r="Y35" s="15" t="n">
+      <c r="Y35" s="9" t="n">
         <v>153787934.235354</v>
       </c>
-      <c r="Z35" s="15" t="n">
+      <c r="Z35" s="9" t="n">
         <v>168701065.6176</v>
       </c>
-      <c r="AA35" s="15" t="n">
+      <c r="AA35" s="9" t="n">
         <v>367214234.446343</v>
       </c>
-      <c r="AB35" s="15" t="n">
+      <c r="AB35" s="9" t="n">
         <v>384718922.536547</v>
       </c>
-      <c r="AC35" s="15" t="n">
+      <c r="AC35" s="9" t="n">
         <v>333792378.138851</v>
       </c>
-      <c r="AD35" s="15" t="n">
+      <c r="AD35" s="9" t="n">
         <v>356041881.589343</v>
       </c>
-      <c r="AE35" s="15" t="n">
+      <c r="AE35" s="9" t="n">
         <v>643485539.1533</v>
       </c>
-      <c r="AF35" s="15"/>
+      <c r="AF35" s="9"/>
     </row>
     <row r="36">
       <c r="A36" t="str">
@@ -6262,16 +6262,16 @@
       <c r="B36" t="str">
         <f>N36</f>
       </c>
-      <c r="C36" s="15" t="str">
+      <c r="C36" s="9" t="str">
         <f>AB36</f>
       </c>
-      <c r="D36" s="15" t="str">
+      <c r="D36" s="9" t="str">
         <f>AD36</f>
       </c>
-      <c r="E36" s="15" t="str">
+      <c r="E36" s="9" t="str">
         <f>AE36</f>
       </c>
-      <c r="F36" s="15" t="str">
+      <c r="F36" s="9" t="str">
         <f>AF36</f>
       </c>
       <c r="G36" s="3" t="str">
@@ -6295,58 +6295,58 @@
       <c r="N36" t="s">
         <v>40</v>
       </c>
-      <c r="O36" s="15" t="n">
+      <c r="O36" s="9" t="n">
         <v>20096300367.6935</v>
       </c>
-      <c r="P36" s="15" t="n">
+      <c r="P36" s="9" t="n">
         <v>15985104110.2386</v>
       </c>
-      <c r="Q36" s="15" t="n">
+      <c r="Q36" s="9" t="n">
         <v>11051301679.3354</v>
       </c>
-      <c r="R36" s="15" t="n">
+      <c r="R36" s="9" t="n">
         <v>6861428245.02892</v>
       </c>
-      <c r="S36" s="15" t="n">
+      <c r="S36" s="9" t="n">
         <v>5271068833.92491</v>
       </c>
-      <c r="T36" s="15" t="n">
+      <c r="T36" s="9" t="n">
         <v>4021994395.74978</v>
       </c>
-      <c r="U36" s="15" t="n">
+      <c r="U36" s="9" t="n">
         <v>3126995890.51699</v>
       </c>
-      <c r="V36" s="15" t="n">
+      <c r="V36" s="9" t="n">
         <v>2252672586.07337</v>
       </c>
-      <c r="W36" s="15" t="n">
+      <c r="W36" s="9" t="n">
         <v>3694564821.21213</v>
       </c>
-      <c r="X36" s="15" t="n">
+      <c r="X36" s="9" t="n">
         <v>2335910588.75374</v>
       </c>
-      <c r="Y36" s="15" t="n">
+      <c r="Y36" s="9" t="n">
         <v>1989770046.28798</v>
       </c>
-      <c r="Z36" s="15" t="n">
+      <c r="Z36" s="9" t="n">
         <v>1861486719.65612</v>
       </c>
-      <c r="AA36" s="15" t="n">
+      <c r="AA36" s="9" t="n">
         <v>2053060235.57906</v>
       </c>
-      <c r="AB36" s="15" t="n">
+      <c r="AB36" s="9" t="n">
         <v>2392550762.45325</v>
       </c>
-      <c r="AC36" s="15" t="n">
+      <c r="AC36" s="9" t="n">
         <v>1865254916.5128</v>
       </c>
-      <c r="AD36" s="15" t="n">
+      <c r="AD36" s="9" t="n">
         <v>2045132368.81667</v>
       </c>
-      <c r="AE36" s="15" t="n">
+      <c r="AE36" s="9" t="n">
         <v>4349132039.113</v>
       </c>
-      <c r="AF36" s="15"/>
+      <c r="AF36" s="9"/>
     </row>
     <row r="37">
       <c r="A37" t="str">
@@ -6355,16 +6355,16 @@
       <c r="B37" t="str">
         <f>N37</f>
       </c>
-      <c r="C37" s="15" t="str">
+      <c r="C37" s="9" t="str">
         <f>AB37</f>
       </c>
-      <c r="D37" s="15" t="str">
+      <c r="D37" s="9" t="str">
         <f>AD37</f>
       </c>
-      <c r="E37" s="15" t="str">
+      <c r="E37" s="9" t="str">
         <f>AE37</f>
       </c>
-      <c r="F37" s="15" t="str">
+      <c r="F37" s="9" t="str">
         <f>AF37</f>
       </c>
       <c r="G37" s="3" t="str">
@@ -6388,58 +6388,58 @@
       <c r="N37" t="s">
         <v>43</v>
       </c>
-      <c r="O37" s="15" t="n">
+      <c r="O37" s="9" t="n">
         <v>143479181461.936</v>
       </c>
-      <c r="P37" s="15" t="n">
+      <c r="P37" s="9" t="n">
         <v>162285532497.217</v>
       </c>
-      <c r="Q37" s="15" t="n">
+      <c r="Q37" s="9" t="n">
         <v>151402719640.374</v>
       </c>
-      <c r="R37" s="15" t="n">
+      <c r="R37" s="9" t="n">
         <v>98686426118.2673</v>
       </c>
-      <c r="S37" s="15" t="n">
+      <c r="S37" s="9" t="n">
         <v>68088344197.2389</v>
       </c>
-      <c r="T37" s="15" t="n">
+      <c r="T37" s="9" t="n">
         <v>41771183380.3403</v>
       </c>
-      <c r="U37" s="15" t="n">
+      <c r="U37" s="9" t="n">
         <v>23611958483.8687</v>
       </c>
-      <c r="V37" s="15" t="n">
+      <c r="V37" s="9" t="n">
         <v>19683614119.4291</v>
       </c>
-      <c r="W37" s="15" t="n">
+      <c r="W37" s="9" t="n">
         <v>14669700733.9954</v>
       </c>
-      <c r="X37" s="15" t="n">
+      <c r="X37" s="9" t="n">
         <v>12763233150.483</v>
       </c>
-      <c r="Y37" s="15" t="n">
+      <c r="Y37" s="9" t="n">
         <v>14622365123.9462</v>
       </c>
-      <c r="Z37" s="15" t="n">
+      <c r="Z37" s="9" t="n">
         <v>13899501665.9389</v>
       </c>
-      <c r="AA37" s="15" t="n">
+      <c r="AA37" s="9" t="n">
         <v>12297973986.1974</v>
       </c>
-      <c r="AB37" s="15" t="n">
+      <c r="AB37" s="9" t="n">
         <v>14126333483.4409</v>
       </c>
-      <c r="AC37" s="15" t="n">
+      <c r="AC37" s="9" t="n">
         <v>13354299200.0388</v>
       </c>
-      <c r="AD37" s="15" t="n">
+      <c r="AD37" s="9" t="n">
         <v>11840793146.6593</v>
       </c>
-      <c r="AE37" s="15" t="n">
+      <c r="AE37" s="9" t="n">
         <v>26136114722.1225</v>
       </c>
-      <c r="AF37" s="15"/>
+      <c r="AF37" s="9"/>
     </row>
     <row r="38">
       <c r="A38" t="str">
@@ -6448,16 +6448,16 @@
       <c r="B38" t="str">
         <f>N38</f>
       </c>
-      <c r="C38" s="15" t="str">
+      <c r="C38" s="9" t="str">
         <f>AB38</f>
       </c>
-      <c r="D38" s="15" t="str">
+      <c r="D38" s="9" t="str">
         <f>AD38</f>
       </c>
-      <c r="E38" s="15" t="str">
+      <c r="E38" s="9" t="str">
         <f>AE38</f>
       </c>
-      <c r="F38" s="15" t="str">
+      <c r="F38" s="9" t="str">
         <f>AF38</f>
       </c>
       <c r="G38" s="3" t="str">
@@ -6481,58 +6481,58 @@
       <c r="N38" t="s">
         <v>40</v>
       </c>
-      <c r="O38" s="15" t="n">
+      <c r="O38" s="9" t="n">
         <v>12022480453.7951</v>
       </c>
-      <c r="P38" s="15" t="n">
+      <c r="P38" s="9" t="n">
         <v>12049860723.0378</v>
       </c>
-      <c r="Q38" s="15" t="n">
+      <c r="Q38" s="9" t="n">
         <v>11247987124.3276</v>
       </c>
-      <c r="R38" s="15" t="n">
+      <c r="R38" s="9" t="n">
         <v>8172686625.05649</v>
       </c>
-      <c r="S38" s="15" t="n">
+      <c r="S38" s="9" t="n">
         <v>6589314445.61342</v>
       </c>
-      <c r="T38" s="15" t="n">
+      <c r="T38" s="9" t="n">
         <v>6326764311.43694</v>
       </c>
-      <c r="U38" s="15" t="n">
+      <c r="U38" s="9" t="n">
         <v>4577289622.84308</v>
       </c>
-      <c r="V38" s="15" t="n">
+      <c r="V38" s="9" t="n">
         <v>5083634552.55849</v>
       </c>
-      <c r="W38" s="15" t="n">
+      <c r="W38" s="9" t="n">
         <v>4559684889.38713</v>
       </c>
-      <c r="X38" s="15" t="n">
+      <c r="X38" s="9" t="n">
         <v>5623018463.65801</v>
       </c>
-      <c r="Y38" s="15" t="n">
+      <c r="Y38" s="9" t="n">
         <v>6669796283.48998</v>
       </c>
-      <c r="Z38" s="15" t="n">
+      <c r="Z38" s="9" t="n">
         <v>7886424223.58715</v>
       </c>
-      <c r="AA38" s="15" t="n">
+      <c r="AA38" s="9" t="n">
         <v>8176886977.35642</v>
       </c>
-      <c r="AB38" s="15" t="n">
+      <c r="AB38" s="9" t="n">
         <v>8054334488.32494</v>
       </c>
-      <c r="AC38" s="15" t="n">
+      <c r="AC38" s="9" t="n">
         <v>7985882603.63557</v>
       </c>
-      <c r="AD38" s="15" t="n">
+      <c r="AD38" s="9" t="n">
         <v>7077283089.4875</v>
       </c>
-      <c r="AE38" s="15" t="n">
+      <c r="AE38" s="9" t="n">
         <v>8611322470.3826</v>
       </c>
-      <c r="AF38" s="15"/>
+      <c r="AF38" s="9"/>
     </row>
     <row r="39">
       <c r="A39" t="str">
@@ -6541,16 +6541,16 @@
       <c r="B39" t="str">
         <f>N39</f>
       </c>
-      <c r="C39" s="15" t="str">
+      <c r="C39" s="9" t="str">
         <f>AB39</f>
       </c>
-      <c r="D39" s="15" t="str">
+      <c r="D39" s="9" t="str">
         <f>AD39</f>
       </c>
-      <c r="E39" s="15" t="str">
+      <c r="E39" s="9" t="str">
         <f>AE39</f>
       </c>
-      <c r="F39" s="15" t="str">
+      <c r="F39" s="9" t="str">
         <f>AF39</f>
       </c>
       <c r="G39" s="3" t="str">
@@ -6574,58 +6574,58 @@
       <c r="N39" t="s">
         <v>43</v>
       </c>
-      <c r="O39" s="15" t="n">
+      <c r="O39" s="9" t="n">
         <v>16704124189.3925</v>
       </c>
-      <c r="P39" s="15" t="n">
+      <c r="P39" s="9" t="n">
         <v>15597127368.5026</v>
       </c>
-      <c r="Q39" s="15" t="n">
+      <c r="Q39" s="9" t="n">
         <v>16161596635.648</v>
       </c>
-      <c r="R39" s="15" t="n">
+      <c r="R39" s="9" t="n">
         <v>13562805723.1655</v>
       </c>
-      <c r="S39" s="15" t="n">
+      <c r="S39" s="9" t="n">
         <v>18630934397.7486</v>
       </c>
-      <c r="T39" s="15" t="n">
+      <c r="T39" s="9" t="n">
         <v>17330589725.2876</v>
       </c>
-      <c r="U39" s="15" t="n">
+      <c r="U39" s="9" t="n">
         <v>15424782688.6793</v>
       </c>
-      <c r="V39" s="15" t="n">
+      <c r="V39" s="9" t="n">
         <v>15315169438.5208</v>
       </c>
-      <c r="W39" s="15" t="n">
+      <c r="W39" s="9" t="n">
         <v>14986877587.8788</v>
       </c>
-      <c r="X39" s="15" t="n">
+      <c r="X39" s="9" t="n">
         <v>15197428239.4648</v>
       </c>
-      <c r="Y39" s="15" t="n">
+      <c r="Y39" s="9" t="n">
         <v>15382007304.9791</v>
       </c>
-      <c r="Z39" s="15" t="n">
+      <c r="Z39" s="9" t="n">
         <v>19031457021.5862</v>
       </c>
-      <c r="AA39" s="15" t="n">
+      <c r="AA39" s="9" t="n">
         <v>18770194772.1515</v>
       </c>
-      <c r="AB39" s="15" t="n">
+      <c r="AB39" s="9" t="n">
         <v>17899248912.8761</v>
       </c>
-      <c r="AC39" s="15" t="n">
+      <c r="AC39" s="9" t="n">
         <v>15709581363.1484</v>
       </c>
-      <c r="AD39" s="15" t="n">
+      <c r="AD39" s="9" t="n">
         <v>15412335206.8195</v>
       </c>
-      <c r="AE39" s="15" t="n">
+      <c r="AE39" s="9" t="n">
         <v>11028697994.0188</v>
       </c>
-      <c r="AF39" s="15"/>
+      <c r="AF39" s="9"/>
     </row>
     <row r="40">
       <c r="A40" t="str">
@@ -6634,16 +6634,16 @@
       <c r="B40" t="str">
         <f>N40</f>
       </c>
-      <c r="C40" s="15" t="str">
+      <c r="C40" s="9" t="str">
         <f>AB40</f>
       </c>
-      <c r="D40" s="15" t="str">
+      <c r="D40" s="9" t="str">
         <f>AD40</f>
       </c>
-      <c r="E40" s="15" t="str">
+      <c r="E40" s="9" t="str">
         <f>AE40</f>
       </c>
-      <c r="F40" s="15" t="str">
+      <c r="F40" s="9" t="str">
         <f>AF40</f>
       </c>
       <c r="G40" s="3" t="str">
@@ -6667,58 +6667,58 @@
       <c r="N40" t="s">
         <v>40</v>
       </c>
-      <c r="O40" s="15" t="n">
+      <c r="O40" s="9" t="n">
         <v>116279253.77012</v>
       </c>
-      <c r="P40" s="15" t="n">
+      <c r="P40" s="9" t="n">
         <v>2745094225.45514</v>
       </c>
-      <c r="Q40" s="15" t="n">
+      <c r="Q40" s="9" t="n">
         <v>2393706848.21061</v>
       </c>
-      <c r="R40" s="15" t="n">
+      <c r="R40" s="9" t="n">
         <v>1833565961.51133</v>
       </c>
-      <c r="S40" s="15" t="n">
+      <c r="S40" s="9" t="n">
         <v>1474255297.22779</v>
       </c>
-      <c r="T40" s="15" t="n">
+      <c r="T40" s="9" t="n">
         <v>744126667.930949</v>
       </c>
-      <c r="U40" s="15" t="n">
+      <c r="U40" s="9" t="n">
         <v>514820985.594724</v>
       </c>
-      <c r="V40" s="15" t="n">
+      <c r="V40" s="9" t="n">
         <v>449721361.009705</v>
       </c>
-      <c r="W40" s="15" t="n">
+      <c r="W40" s="9" t="n">
         <v>441688712.505163</v>
       </c>
-      <c r="X40" s="15" t="n">
+      <c r="X40" s="9" t="n">
         <v>584800479.861838</v>
       </c>
-      <c r="Y40" s="15" t="n">
+      <c r="Y40" s="9" t="n">
         <v>288060577.024133</v>
       </c>
-      <c r="Z40" s="15" t="n">
+      <c r="Z40" s="9" t="n">
         <v>333728994.50215</v>
       </c>
-      <c r="AA40" s="15" t="n">
+      <c r="AA40" s="9" t="n">
         <v>489472944.550697</v>
       </c>
-      <c r="AB40" s="15" t="n">
+      <c r="AB40" s="9" t="n">
         <v>327876440.045681</v>
       </c>
-      <c r="AC40" s="15" t="n">
+      <c r="AC40" s="9" t="n">
         <v>294904664.842728</v>
       </c>
-      <c r="AD40" s="15" t="n">
+      <c r="AD40" s="9" t="n">
         <v>260661377.308312</v>
       </c>
-      <c r="AE40" s="15" t="n">
+      <c r="AE40" s="9" t="n">
         <v>1719360865.2598</v>
       </c>
-      <c r="AF40" s="15"/>
+      <c r="AF40" s="9"/>
     </row>
     <row r="41">
       <c r="A41" t="str">
@@ -6727,16 +6727,16 @@
       <c r="B41" t="str">
         <f>N41</f>
       </c>
-      <c r="C41" s="15" t="str">
+      <c r="C41" s="9" t="str">
         <f>AB41</f>
       </c>
-      <c r="D41" s="15" t="str">
+      <c r="D41" s="9" t="str">
         <f>AD41</f>
       </c>
-      <c r="E41" s="15" t="str">
+      <c r="E41" s="9" t="str">
         <f>AE41</f>
       </c>
-      <c r="F41" s="15" t="str">
+      <c r="F41" s="9" t="str">
         <f>AF41</f>
       </c>
       <c r="G41" s="3" t="str">
@@ -6760,58 +6760,58 @@
       <c r="N41" t="s">
         <v>43</v>
       </c>
-      <c r="O41" s="15" t="n">
+      <c r="O41" s="9" t="n">
         <v>1135565293.06255</v>
       </c>
-      <c r="P41" s="15" t="n">
+      <c r="P41" s="9" t="n">
         <v>8651533051.52256</v>
       </c>
-      <c r="Q41" s="15" t="n">
+      <c r="Q41" s="9" t="n">
         <v>12319288525.5392</v>
       </c>
-      <c r="R41" s="15" t="n">
+      <c r="R41" s="9" t="n">
         <v>4130914997.79964</v>
       </c>
-      <c r="S41" s="15" t="n">
+      <c r="S41" s="9" t="n">
         <v>2979356320.93152</v>
       </c>
-      <c r="T41" s="15" t="n">
+      <c r="T41" s="9" t="n">
         <v>2446786154.25965</v>
       </c>
-      <c r="U41" s="15" t="n">
+      <c r="U41" s="9" t="n">
         <v>1391834451.67874</v>
       </c>
-      <c r="V41" s="15" t="n">
+      <c r="V41" s="9" t="n">
         <v>1222394413.80361</v>
       </c>
-      <c r="W41" s="15" t="n">
+      <c r="W41" s="9" t="n">
         <v>856385141.561649</v>
       </c>
-      <c r="X41" s="15" t="n">
+      <c r="X41" s="9" t="n">
         <v>808011240.718388</v>
       </c>
-      <c r="Y41" s="15" t="n">
+      <c r="Y41" s="9" t="n">
         <v>916803226.499431</v>
       </c>
-      <c r="Z41" s="15" t="n">
+      <c r="Z41" s="9" t="n">
         <v>871623914.090263</v>
       </c>
-      <c r="AA41" s="15" t="n">
+      <c r="AA41" s="9" t="n">
         <v>1049308363.74618</v>
       </c>
-      <c r="AB41" s="15" t="n">
+      <c r="AB41" s="9" t="n">
         <v>928095514.024027</v>
       </c>
-      <c r="AC41" s="15" t="n">
+      <c r="AC41" s="9" t="n">
         <v>432279122.064571</v>
       </c>
-      <c r="AD41" s="15" t="n">
+      <c r="AD41" s="9" t="n">
         <v>480686438.079784</v>
       </c>
-      <c r="AE41" s="15" t="n">
+      <c r="AE41" s="9" t="n">
         <v>1783365852.8155</v>
       </c>
-      <c r="AF41" s="15"/>
+      <c r="AF41" s="9"/>
     </row>
     <row r="42">
       <c r="A42" t="str">
@@ -6820,16 +6820,16 @@
       <c r="B42" t="str">
         <f>N42</f>
       </c>
-      <c r="C42" s="15" t="str">
+      <c r="C42" s="9" t="str">
         <f>AB42</f>
       </c>
-      <c r="D42" s="15" t="str">
+      <c r="D42" s="9" t="str">
         <f>AD42</f>
       </c>
-      <c r="E42" s="15" t="str">
+      <c r="E42" s="9" t="str">
         <f>AE42</f>
       </c>
-      <c r="F42" s="15" t="str">
+      <c r="F42" s="9" t="str">
         <f>AF42</f>
       </c>
       <c r="G42" s="3" t="str">
@@ -6853,58 +6853,58 @@
       <c r="N42" t="s">
         <v>19</v>
       </c>
-      <c r="O42" s="15" t="str">
+      <c r="O42" s="9" t="str">
         <f>Sum(O24:O41)</f>
       </c>
-      <c r="P42" s="15" t="str">
+      <c r="P42" s="9" t="str">
         <f>Sum(P24:P41)</f>
       </c>
-      <c r="Q42" s="15" t="str">
+      <c r="Q42" s="9" t="str">
         <f>Sum(Q24:Q41)</f>
       </c>
-      <c r="R42" s="15" t="str">
+      <c r="R42" s="9" t="str">
         <f>Sum(R24:R41)</f>
       </c>
-      <c r="S42" s="15" t="str">
+      <c r="S42" s="9" t="str">
         <f>Sum(S24:S41)</f>
       </c>
-      <c r="T42" s="15" t="str">
+      <c r="T42" s="9" t="str">
         <f>Sum(T24:T41)</f>
       </c>
-      <c r="U42" s="15" t="str">
+      <c r="U42" s="9" t="str">
         <f>Sum(U24:U41)</f>
       </c>
-      <c r="V42" s="15" t="str">
+      <c r="V42" s="9" t="str">
         <f>Sum(V24:V41)</f>
       </c>
-      <c r="W42" s="15" t="str">
+      <c r="W42" s="9" t="str">
         <f>Sum(W24:W41)</f>
       </c>
-      <c r="X42" s="15" t="str">
+      <c r="X42" s="9" t="str">
         <f>Sum(X24:X41)</f>
       </c>
-      <c r="Y42" s="15" t="str">
+      <c r="Y42" s="9" t="str">
         <f>Sum(Y24:Y41)</f>
       </c>
-      <c r="Z42" s="15" t="str">
+      <c r="Z42" s="9" t="str">
         <f>Sum(Z24:Z41)</f>
       </c>
-      <c r="AA42" s="15" t="str">
+      <c r="AA42" s="9" t="str">
         <f>Sum(AA24:AA41)</f>
       </c>
-      <c r="AB42" s="15" t="str">
+      <c r="AB42" s="9" t="str">
         <f>Sum(AB24:AB41)</f>
       </c>
-      <c r="AC42" s="15" t="str">
+      <c r="AC42" s="9" t="str">
         <f>Sum(AC24:AC41)</f>
       </c>
-      <c r="AD42" s="15" t="str">
+      <c r="AD42" s="9" t="str">
         <f>Sum(AD24:AD41)</f>
       </c>
-      <c r="AE42" s="15" t="str">
+      <c r="AE42" s="9" t="str">
         <f>Sum(AE24:AE41)</f>
       </c>
-      <c r="AF42" s="15"/>
+      <c r="AF42" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>